<commit_message>
Salva as informações desejadas em um excel
</commit_message>
<xml_diff>
--- a/FiltroOtimoContinuo/ErroEstimacao/ErroEstimacao_J7.xlsx
+++ b/FiltroOtimoContinuo/ErroEstimacao/ErroEstimacao_J7.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:F3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,6 +433,77 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ocupacao</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Pesos</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Matriz_Covariancia</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Erro_Estimacao_Amplitude</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Media_Erro_Estimacao</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Desvio_Padrao_Erro_Estimacao</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[-0.14339454108469085, 0.11960066703238818, -0.9949803054570084, 2.1723204512071397, -1.4340851491821278, 0.670651331924537, -0.3901124544402377]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[[ 5.05233430e+02  3.59521213e+02  1.41835422e+02  3.72691888e+01
+   7.31522850e+00  9.03398774e-01 -4.08527618e-02]
+ [ 3.59521213e+02  4.98091789e+02  3.55207374e+02  1.41522106e+02
+   3.84938636e+01  7.45866855e+00 -1.37401295e-01]
+ [ 1.41835422e+02  3.55207374e+02  5.02425347e+02  3.62997103e+02
+   1.44129886e+02  3.69871686e+01  5.32898808e+00]
+ [ 3.72691888e+01  1.41522106e+02  3.62997103e+02  5.13320673e+02
+   3.65379898e+02  1.43639191e+02  3.77415259e+01]
+ [ 7.31522850e+00  3.84938636e+01  1.44129886e+02  3.65379898e+02
+   5.09426324e+02  3.64256507e+02  1.45017509e+02]
+ [ 9.03398774e-01  7.45866855e+00  3.69871686e+01  1.43639191e+02
+   3.64256507e+02  5.10482666e+02  3.62599296e+02]
+ [-4.08527618e-02 -1.37401295e-01  5.32898808e+00  3.77415259e+01
+   1.45017509e+02  3.62599296e+02  5.03142586e+02]]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[10.963804422385438, -6.419417684714378, 8.591147980621551, -6.909173094399636, 6.654634230543489, 0.262950001603334, -2.3177950756164174, 3.7949114617889412, -1.6758122559240234, -0.029768978717908068, 4.014176256208368, -0.9531122546353448, 7.093454556998203, 53.809865849359056, 26.653957798671954, 51.39348811293895, 32.65744510146598, 3.986092007957211, -11.813679641368909, 86.96642169430693, 61.99121724958726, 61.417224694271965, 11.369343236079029, 9.447396359588822, 8.61314094119848, 25.32722868710443, 30.528222848148417, 20.841381471268022, 10.210560744143208, -1.3980847546838024, 3.0695674465896143, -1.7747976561966217, 2.849855725199466, -2.6821364788362145, -1.948949774707485, 4.445174069940222, -5.658129696904189, 8.48745064910769, -10.124341229837459, 7.4579893792946, -2.8412299537658567, 28.456181601917823, 2.1479150205755317, 33.386754324713294, -1.9809703549019524, 26.877139382619774, 16.114128071228883, 51.87593141529892, 45.102299909789245, 91.71878799623234, 11.161513049923286, 133.0313549697823, 27.40504829822924, 27.94219753824035, 19.413164710834977, 98.85967729254322, 58.841096079212846, 23.334583072972336, 27.11674883890105, 7.231341266378159, 10.258779876908426, -1.6383544817196705, 5.483560648565518, -6.949225144983137, 8.812122051453294, 4.144210959939853, -2.9228163298876346, 14.054664552093346, -1.7249108508642053, -5.383841276492426, 4.067849440687723, 13.507613145109124, -6.239086167997154, 11.196909574010197, 20.29758595259385, 45.83399742016664, 7.228271877745925, 77.14311603227831, 8.782752268058772, -56.23847402274225, 51.195354044877654, 36.25364199684658, 25.42629073635089, 4.614173131366974, 4.788709500316826, -6.131101580910678, 4.216078748321351, 1.673180712322694, -3.7319317192988604, 0.2869401106253251, 1.2170301550327969, -3.439595722250816, 5.236145183917018, -2.726723600739994, 0.7471836172418019, -0.35633697779790724, -0.8348389050712577, 11.563735978989609, 8.43116536373828, 10.21139124141288, 20.340191683038455, -8.980877997315247, -1.2877298031584434, 6.787924533090226, 16.11081108233159, 8.223501755668778, 0.25100628214789794, 9.03151345742128, 6.856848348827693, 9.189043765223737, 20.412357633740015, 9.87368589093272, -22.24069357626605, 62.370558334509944, 36.231491249304966, 47.77771314552982, 41.07970174719967, -3.762467673612946, -13.899823846511211, 55.58210719170114, 35.79237150453775, 25.734854746506308, 1.7283701142715777, 4.801524699697631, -3.0125563251688154, -0.3329854163150259, 4.434475812580423, -1.4439573561749208, 8.703206816959497, 20.516922578258086, 5.906729985283036, 51.85206489444627, 36.45584835106372, 44.662513541873935, 55.65374284175736, 68.51504856694851, 5.104824859852869, 97.5284459181121, 73.5537785569966, 50.73627304671919, 2.6719362137107785, 62.085451968506376, 10.530828941196406, 33.03751743589956, 12.513477432249408, 20.226193963860318, 26.211197816677437, 19.233770498037586, 85.33300660636833, 18.2933030828992, 45.451180474899104, 0.671116113184155, 52.57744695599746, 22.740238178649587, 49.63775479007014, 47.3898186327428, 36.65153764112745, 37.979384947799694, 13.109728578987514, 38.257537678349536, 1.5953853616442046, -14.660526752895265, 66.48422293440566, 34.95657838786495, 34.43649749190274, 61.4841918448967, 68.36359935155949, 12.720756360771759, 134.96793979080866, 48.82213073925834, -50.428727803547105, 108.70884680164113, 38.73886873340189, 34.06583296633009, 24.597870065515718, 23.642155689697226, 11.227681205848034, 14.480429579338235, -2.3730794373736224, 5.53713319237124, 9.62323198415842, -3.9005252955596346, 2.8127587802556278, -6.89976918044721, 11.784067461410968, -3.027320327842644, 6.339343088582748, 23.758778625798474, 2.725419172498185, 28.42679655385639, -6.642065378407965, 4.5081557348771355, 6.51810031100843, 20.862940886987168, 14.352708767816798, 7.957536399803486, 1.763030785883009, -3.611079014369215, 9.275054100954812, 0.8032161810131715, 10.864302880382471, 10.20677393076912, 49.111447993594545, 37.3803474218615, 3.164461246587912, 81.80963387984023, 26.01106671046489, -54.786040580160325, 60.841619613837494, 30.428102622828405, 29.214102009818433, 14.372792887768673, 1.9236117359083167, 22.51002096123455, -5.6537346367639945, -0.8064812234167817, 5.1214371384684485, 7.672238602637837, 11.560652172435788, 2.6746901454245195, 0.16811660915466708, 5.46471290261834, 1.6858156400159823, 0.4288935179988598, 4.349143124932903, -4.8497480847844, 5.107480622743742, 3.827691185073015, 3.864022930698831, 1.7303702624289046, 2.7816986253773437, 1.7622950886711932, 0.9154552685812831, -2.6956466942265136, 1.9077778718086607, 2.8922364505300115, 1.9971651505634354, 1.5894752422200473, 14.12772872945139, 0.14220393286140975, 24.063877286073797, -7.6034401507461205, 13.67269665423968, 0.5119917134309315, 12.765007901164953, 8.305583869982264, 47.455628712492356, 22.69594376558142, 35.717158013867966, 26.449702100859184, 0.32679382525449796, -14.342018235891063, 44.26309187426695, 27.269380666876728, 18.92661740337368, 6.5904982134509, -1.942846485640219, 5.2978896246523846, 26.592667837472824, 18.122784342488572, 26.61161192944742, 22.87348069014812, 29.50555635971878, 13.991792584531545, 64.70106156297116, 62.4952942792778, -5.7429396318964905, 19.95763544769794, 29.646249659004283, 41.09474068066718, 24.92590090935548, 9.090439126403512, 9.969289584845132, 4.111122531819541, 21.643070320056726, -4.564298110319754, 26.159065590953563, 12.22646466425677, 20.641584570725982, 39.19203245692782, 13.01443498809456, 14.332250716611682, 3.5725477942432264, 44.16978156079248, 39.10987424348361, 17.50803219753817, 44.82933776563355, 9.381375446574694, -37.81055168109461, 36.069606458521115, 7.480051561439793, 22.674391953409554, -3.4254575465872357, 6.7797013998456555, -1.339268288830581, -2.030867217461452, 7.941542608092689, -13.50057476111568, 9.925101253132055, 1.7699695493157392, 18.632801274711113, 2.6255934973794197, 24.48206139124677, 2.889902768331595, -22.73610868080233, 25.546249644461184, 9.944702647763862, 17.93404062627791, 7.322012451263397, 19.831283322910842, 51.53835767337931, 14.881030571421562, 66.17775624563444, -8.726691356930354, 26.29572142072027, 16.01075050272229, 58.66326255545397, 36.521781330232265, 27.306187925251752, 27.779316302747702, 10.223999069751343, 29.062581476765708, -2.2058410822553967, -3.4011319345563606, 20.592567103897732, 17.367627671341747, 14.27872314897354, 9.381297993811822, -1.8555961246797155, 1.212212324974744, -0.18376428570115602, 1.2522895030552288, -3.029845853588345, 4.618541348781362, 18.54151005321054, 38.92740179276902, 25.3868076120717, 55.67275137323004, 14.258622151404339, -15.611362023552203, 34.89151751140287, 56.451292542961895, 57.01302809495756, 14.311724909377462, 2.1675148696117077, 3.0636097837153784, 29.121419313641276, 14.374953197742647, 31.9358115547629, 32.66001453974671, 9.403567526705494, 61.150499280172184, 4.701128658043899, -48.97986299924297, 45.82242525035449, 27.09774706853283, 15.057403491709286, 10.963486276871636, -3.841606962764413, 3.300642101360493, -0.9812985578081236, -1.9386700837531026, 1.5062811466568613, 4.318209413802614, 9.489993676296358, 14.264017129042365, 26.205408731762304, 21.18373190421681, 17.410472521219603, -19.85809410459829, 27.102376255896814, 25.86063759110166, 18.609492222317357, 43.451259461102964, 20.72249610425556, 16.235047370378147, 47.02050550851601, 8.342255917540342, -30.76337992519582, 41.263987126914564, 21.70091225107124, 42.42181796268072, 28.561534569973446, 24.858494627954002, 30.926734941137198, 0.8130217980017278, -18.91598511788269, 48.08167568506626, 51.714072243114124, 32.04211352896489, 36.47068295764774, -6.188925082967806, 4.691521740657464, 35.31951688104043, 45.03630853570855, 42.87085869824372, 16.397498805789027, 4.946714936871729, -4.514589879289554, 33.30150219693623, 14.612217262830415, 18.425109179406196, 16.854963566938622, 7.326099128849769, 17.421160093010258, 18.173884575885047, -2.783647168005004, -11.446108290072482, 24.228234091954267, 11.133028841824366, 31.859562417846213, 8.329491705456217, 31.102755417530652, -2.7124313338280004, 4.340950314098947, 4.115427660831929, 21.111264105042434, 16.29684613313592, 8.594879358757913, 4.7723524280366, 1.0960914346803592, 0.6307536665499364, 14.563679985686496, 7.6856163317956785, 14.166667443780295, 14.946205631332814, 0.18711464265571465, -8.996668696445509, 15.312197031972842, 30.02289785122899, 11.120740665612534, 27.198743940369926, 14.069593592029403, 11.399682516770994, 1.5895364751222898, 20.313552641793386, 2.3861631733468935, 19.119742723194296, 12.78668072308835, 4.512044134011193, -1.0509962779359379, 4.867827822838006, 0.7977792968374384, 16.1083911145095, 8.086329875656576, 10.581826120831554, 4.459924834969229, -11.374138399571741, 20.060896043754255, 3.8793189344019323, 7.476330353704768, 7.7675561705809075, -6.311219759104397, 8.177891510411236, -8.700401307650782, 7.185932653436935, -6.967029832405512, 7.19499932160935, 16.816910188496138, 9.797774531589688, 30.031230551656606, -3.2057851528208836, 4.1232926191771355, -1.880598105784996, 27.292589032259293, 12.569544896069628, 7.106430360878286, 5.916512340105086, 4.20236578205249, 62.33133314943409, 24.876747775558243, 98.6698572986256, -4.575486128171008, 32.57203156758396, 50.96485566408073, 64.72139254237442, 45.65309471828126, 55.57142083096507, 71.37510409999456, 32.47352476653593, 85.1955438011851, -34.30211604321703, 21.512767226466593, 48.95341035886932, 69.40768813059566, 70.33743675811593, 44.17444935613969, 1.5516421440417787, -12.731200262664107, 39.33586263105635, 36.467673635472856, 19.927290880127302, 10.10061885720237, 15.967142024803163, -0.9176835209061842, 4.785454586738169, 24.493384706251938, 11.39052641833576, 49.270464824631276, -5.852269263876553, 7.108178018505612, 4.522845043055673, 26.705186805197673, 11.719271188538729, 13.922920993416463, -0.3619554078176276, 3.794967038919492, -2.09594482148852, 0.038212215764959756, 0.7543538390741511, -3.721932903575941, 2.259223920031712, -1.3657481808214091, 5.311392578220338, -0.9563789954061519, -3.383591915898333, -1.4092593992358826, 2.183050112005874, 0.39775715801125244, -0.364427456677652, -0.23373924457681666, 0.9507203273638245, -3.4917064030092178, 2.056750722164607, 2.127247068810753, -1.7500820142228632, 3.061090970143044, -2.560772896933708, -0.5498679837659437, -0.5018550718716269, 0.7194361617006007, 0.18572509208188853, 3.9256757833546114, -5.268733106220703, 3.8296236803907524, -3.186283791111265, 47.92493611795526, 14.390824814891161, 57.18673126386305, 2.36198708940503, 3.4000219800295213, 2.278374976924689, 52.51206325430047, 36.881433036051384, 37.54310961745041, 11.686942417478768, 39.05125208148441, 10.737190277553324, 5.22518932536504, 18.950382225796545, 15.5780513906587, 12.524108107721403, 29.986620808347496, 15.66656466450523, 19.51906952400509, 3.5069212191571992, -0.4757855675860867, 16.339303066191484, 10.965097279066942, 11.49347498978327, -12.716992329905972, 9.969963353292963, 2.9214365857395337, 27.24583566369341, 25.90330038063462, 10.959796244776548, 52.867878039638484, 10.901475625110976, -41.732740084148475, 37.60899443815548, 24.54104491332751, 12.76127706542887, 14.27522726239414, -3.2098397333417488, 3.129460251496576, 0.1895534365347641, -0.8376076255928464, -2.462461138847518, 4.369994230515522, -5.459570012147273, 5.71693745132891, -6.259833151006488, 7.475119153676498, -6.7403976673748405, 4.851161325616529, -2.257730570446203, -2.479309512502845, 16.27965170871085, 2.901442530659949, 12.182093116463511, 12.525761171412885, -2.897325082659222, -6.955689966885845, 17.306880696437773, 5.649888189046847, 9.257683080878788, 2.1893780405379877, 1.5273751315339368, -1.310698509917214, -0.25141499417080093, 0.6502444259078368, 3.7870988453115992, 3.5652523532208678, -0.5729916594838279, 0.35714584649748815, 0.4541811290783624, 7.511882672059571, -4.849462957315222, 19.344810784318987, 3.423564401903633, 74.98481927818568, 89.14330945590538, 26.781905194418428, 132.5068212423966, 39.74379119373174, -109.88155380612822, 118.2481702285384, 67.55819356372366, 50.5207080515278, 33.58246450166527, 21.080671105101707, 16.56595412364965, 27.675908526273606, -3.2446853356833856, -3.9077179371201614, 30.818362045655245, 18.059155420960607, 24.838896306893314, 27.130733500179687, 1.1718980105541021, 36.33779899500191, -3.959806388455533, -14.981409516980822, 83.04345760058146, 34.829640340708565, 85.27128054006693, -6.621536296108122, 3.129578581665214, 16.459954889265614, 63.99621114141256, 40.095735825406784, 27.35293134073448, 11.434376719240841, 0.1664410395961866, 8.752137671236818, 4.660636378766872, 1.6752812508682133, 45.5622847967967, 18.168286504204502, 71.85930317786386, 1.871193364827171, 22.581979688156537, 6.277564022456815, 57.17968529881715, 38.98876576160699, 32.92460729893822, 54.49298216248907, 43.84990721853758, 126.04935821267863, 41.664081563767866, 142.08667202253656, 58.36616538913404, -39.75914258572652, 88.40945079905359, 148.7813657104155, 85.74457806944847, 28.87125846121046, 48.14151308502555, 40.712025156362586, -10.085872142719888, 38.049418492454976, 17.049044310239246, 24.757711725775835, 2.5569053420625387, 21.89464402795654, 1.2175054263138243, 14.746715891822127, -2.865212998948401, -0.7737702481971208, 16.456341858326322, 7.959308532120553, 12.957680245401498, 2.9725822671041495, 4.5218664339816605, -4.935067125612017, 2.2131240325296915, 3.6245355603642193, 1.3804583531960533, 24.496380141047677, 6.786818031962795, 30.11055239010064, -16.295869452957117, 11.166858697453705, 3.110660150521165, 27.407502081054353, 10.59282077863541, 7.393185437824538, 5.507318359147138, 8.042877599767003, 18.85125663903551, 28.370644071068178, 58.73552768045741, 86.97037306782097, 64.30077955005399, 119.04395421576336, 88.01018237952611, 79.91735362287329, 62.02043045737385, 149.8166989125922, 103.6966646773953, 77.70077482884722, -16.774142332553993, 90.0001007452624, 43.620969733449726, 31.09011966476024, 7.050925866751468, 10.27279809445509, 1.0341878690208806, 1.8413396425912634, -7.808699023649386, 13.48723037287959, -8.746408136188661, 9.146486750798845, -5.8782991632518655, 2.245984260020897, 3.3726576826912176, 0.748718881086484, 5.890697553204161, 10.411016195297712, 2.7601259770211364, 1.0762397988680803, -2.8373011882814874, 9.394875088170483, 2.2640258039997105, 8.255417114722412, -5.51876443012742, 7.480362062042602, -7.266961622773849, 9.186070732971494, -11.036386763269944, 8.2739376392174, -3.426411656753448, 1.6347063877521584, 30.558507958212818, 6.056996331385591, 32.50688369480063, 8.045485297318955, 1.2061224922382792, -8.24653392335716, 38.170339729711806, 14.069973250111007, 14.53515590440337, 6.0167530188606015, 43.206175742087005, 34.41234056600142, 37.561419003521216, 51.38165981121489, 5.871981738685577, -43.92262693537896, 72.50348770547032, 33.54159230109732, 30.8326839443879, 8.05989147559968, 2.60969934610743, 26.68877652808804, 11.135594687586135, 29.24222332181554, 14.379621426103682, -2.6603064577872786, -3.076542350633499, 25.9568801029108, 24.083485377784406, 37.40222329671735, 42.09664524782929, 37.04475182550744, 24.141147659240126, 22.415090713392743, 41.40443363472719, 70.8848647443081, 96.37217794447824, 63.81005469959287, -28.091418952441444, 14.713500450022973, 58.348359696537436, 46.376366816073, 29.562994724754226, 15.704569614645688, 23.375071559066097, 12.081660348973386, -1.4230330734703145, 37.517175244411106, 15.805617261165844, 0.5504919767299157, 24.602959543871734, 12.465540852789625, 20.902218287111566, 6.9160621698991935, 2.5991523980431452, -2.0082119480369442, 10.321064592332476, 15.338806685650274, 18.45862196628877, 6.821344339056253, 21.334664381908354, 4.677385872848092, -17.422818727325687, 26.740671598077153, 13.122260728249438, 17.757261979892956, -3.3172038586451422, 13.59330269902419, -12.909784764611548, 16.25724252218062, 3.06806234192549, 2.3215871668116383, -0.18542607949998002, 3.6354894413559293, 54.10550566812083, 61.991470144663595, 32.26556657417687, 122.92062176129146, 30.369965150339226, -98.83442911983367, 101.0378553583163, 70.12373319138246, 34.04583775842246, 12.128679863370477, 12.613450152062498, 6.82980414403246, 8.286031306165425, 6.781535908516424, 34.09516254675364, 40.86478719022034, 12.092013018864272, 65.88195537076346, 4.683202260255598, -8.060493474319646, 56.53340948773249, 62.99678291216307, 41.81712043979095, 28.936226362819582, 78.89283808861954, 83.70874131381474, 44.66326407890307, 92.38777683477234, 44.608673013745715, -22.58546857944628, 83.13056387805715, 37.65904820812647, 45.15834236878267, 33.77396072796406, 19.96137695138697, 22.030273680579263, 11.015547734156767, 7.026780337493264, 4.5518706912210325, 27.537472528181894, 12.237832532110492, 20.70867170300941, -1.510347341614737, 10.778225686203191, 1.7083804020953186, -0.01869015171678895, 0.12935111754559148, 1.108195122777898, 0.8759070893103593, -2.9213331837764165, 1.800146319868821, 6.657890902693673, 21.535511679424964, 1.3918333918494241, 29.310315296108456, 11.592626745703896, -29.987926738694284, 19.720948415139013, 10.075924427262445, 16.95577453610666, -2.961307190545028, 1.603887634048637, 6.172151771516482, -7.571419001200001, 8.643923712403197, 11.64885759750716, 31.476473262337457, 1.5588952798263165, 94.74111457123448, 67.21170103657474, 23.514627414497255, 133.17948651711828, 36.46734109297586, 10.516684614782037, 76.11962348451203, 70.10006646215412, 83.75746776103622, 59.6371345944251, 27.689873853910157, 32.132216432460474, 51.51389906889004, 24.880556919001535, 29.072953722163394, 26.228496994206125, 25.38871828986724, 40.234563980622816, 17.601731490070513, 6.853632712315957, 15.552379085911378, 15.086737955318773, -3.7949097537349252, 5.807741969498272, 2.6092444141494253, -2.5236650273872767, -0.313652376709598, 1.6217185830434797, -2.998734187671086, 5.63992475272879, -1.0724448868000873, -1.3151340588921898, -1.0362558361752228, 0.8267726482017168, 2.4346809754984244, 2.9284784271776996, -4.476455721668018, 5.14196410041807, -5.848238782953469, 20.2472427193008, 7.503363490580735, 43.4332945674136, 41.67058425375028, 35.56174728486343, 35.17944140867541, 37.784325368749876, 0.3188567949374175, 46.00617063276987, 69.40439002678448, 46.62247943554402, 41.26052552633463, 16.58303243169192, -22.684945852814934, 42.2955477129314, 12.33191029785181, 19.75162958413654, -3.4470384410390817, 8.294147140903513, 7.747935142231952, 6.552130642489152, 6.432672373121916, 1.8346242796124343, 2.799378273187912, 1.0551115370000375, -3.7256796723599277, 9.600394337437052, -0.980788974568144, 2.75530549353078, 5.287242036656306, -2.334154124797226, 5.881121098230103, 46.50222926692312, 12.958987865231421, 69.84134752324636, -12.469918320086045, 14.224445483350564, 8.164558324811061, 84.3475879143082, 38.3893166649647, 95.65470120416634, 2.1832530007062303, 73.86242486016297, -16.181083886300577, 39.32713504495533, 27.85352959879806, 48.565184725666654, 29.623747033926584, 33.08370384301778, 8.10345594495031, 12.679402558588482, 7.193041917390195, 4.351938047528677, 7.168231722846757, 17.117574596608396, 7.216575781077054, 2.831210427315554, 6.731950130052189, 6.800909117516573, -0.6487533213572941, 8.199956212972227, -5.000564494756847, 11.446129209292348, -5.741231434894834, 27.50083823117454, -0.03256431681068861, 16.56513004497762, -0.19537019931522526, 2.603253895291843, 9.035976297124169, 12.635875005705671, 14.418750173000687, 1.965008885765979, 0.15283054202871843, 4.502758034331163, 6.454043093352853, 7.963742350028338, 8.027052600914764, 10.967112294295905, -1.2430798571267325, 9.637785107184861, -4.185444591588373, 14.057581237090247, 4.205307322509485, 7.017243538340267, -2.728310162701156, 22.88486646364003, 62.445787169865454, 14.92846924337293, 100.99620624453172, -21.01775646758702, -11.15044046930089, 29.60692127146112, 79.1522449103986, 30.667134507660307, 33.2085825845372, 4.428035421125756, 8.34579839721005, -13.594798608401991, 11.870630835089448, 10.524744505153002, 12.85607548333148, 27.456035792398005, 22.058636447703805, 25.369478407887996, 31.83273816191705, 51.6239107853566, 96.67256936560901, 81.96836966182568, 38.000780842805796, 45.17462656350512, 81.02807589701786, -12.68394152521525, 81.59382369416979, 34.892024252939095, 21.381873093746858, 26.6898730927101, 43.88052032002462, 58.69283858569574, 54.49221359105495, 90.70663429834136, 8.057738525756491, -11.309313322303531, 149.9696988347689, 82.04954840310013, 70.69321799755184, 48.07921836861895, 51.25486691648695, 4.789788441271174, 76.83929269147256, 39.07468499703156, 16.654586750826763, 9.168238978750626, 13.28828219434635, 6.255172248358738, 2.3983693174398235, 0.6226764643217437, 5.010000035402371, -6.603243649643, 8.847824134689734, -2.876810983999812, 0.7289842837420277, -3.279758008755326, 5.220328211977897, 6.045818164917872, 0.8467414303055651, 10.281245726770265, 14.548947996130225, 20.65414895337922, 10.85002491779273, 48.14222919523364, 37.333154111143884, -11.923592311347413, 84.34912259516973, 36.48971880613473, 6.629687128247255, 102.3591405134866, 48.34000550201765, 101.42158253113894, 11.900038937739112, -55.164177107977885, 82.97776500627177, 42.62997530828501, 32.25884538887614, 10.089739839053118, 2.9171849752851178, -1.5054024057408553, 0.9810516970075019, 0.17783921474722353, 2.455688890263451, 2.5209650809638458, 43.67136869689038, 55.41437235759426, 22.932818553781573, 96.35868371238821, 9.747147943375012, -73.1014150786105, 90.85902103779652, 48.625433657605825, 45.742383021999984, 21.96689301306667, 17.178526830136214, 33.4189997729633, 17.83360055052242, -1.2012282113697452, 137.6529493657726, 78.18520718641314, 93.74203968862375, 137.18966810076998, 48.844121850945385, -6.68759587158339, 140.49399980921865, 61.815555091854705, 92.70675957628053, 35.99511904554866, 56.14541511011397, 39.81933510932956, 23.032971849978793, 38.484868807966265, 10.591570008600257, -21.053853002964225, 54.317726981909914, 17.736994007508446, 10.24222477852025, 14.353666201526924, 2.6522529282787515, 7.7936898510074935, 24.295435810543896, 26.765346672818794, 21.000931483121946, 50.10486183278114, -11.208611569072204, -10.404789846072106, 32.854852725233535, 34.53332998120255, 20.54591174808724, 15.048224903140508, -5.719938754180203, 8.648548614259598, 6.704276487626362, 11.747295787191081, 7.869879894559801, 18.43688919209728, 0.481985055793956, -14.613247780029923, 20.571616697026695, 8.738871127355821, 5.450928259405285, 4.454183167999255, -1.8926422365657665, 35.211512271180766, 16.134215741640418, 34.689377645757965, 17.31862858438992, 5.757139426675138, 7.936813467215693, 60.549662952987575, 59.97838400928519, 46.785473248181134, -5.759589951209215, 26.451987729513107, 11.585024235400546, 39.45981654852574, 54.55049304579518, 42.50165691823445, 53.50420620296736, 36.54001488731066, -14.457335163962142, 22.99693410426017, 15.874055394573483, 43.86531070314011, 18.998111027559478, 10.216708714382515, -2.1688154630695147, 9.30722706654009, -6.86186042810584, 4.194115990233447, 2.4104280459755283, 5.949323180192973, 1.7396956994814392, 12.342563462758726, -6.853514567646357, 5.794459899484764, -4.276905120697153, 16.7451891751795, -3.1887387927617126, 4.931128976121094, -4.047461569276654, 1.2256132895263046, 1.3845217294259675, -2.4414264424521335, 4.031243450889584, -5.647855401984925, 2.705870975747417, -0.927362293507838, -1.3579713026872344, 4.83524709778491, -3.706493353178872, 5.662867262929591, -3.8645897750975413, -4.277185248832327, 5.256281878860347, -1.3792776923857717, -1.5153871093967497, 20.43606059806084, 2.1423425907507117, 17.261314320142652, 14.343504929507482, 37.501092170756706, 43.42733246372812, 33.239205758811735, 110.4293122212254, 18.38992259318576, -73.81680759690288, 94.61169623650461, 38.88785958826219, 61.8586380765901, -1.7725944891724055, 13.985122702558229, -1.3917958749710468, 27.50634331359692, 7.073048414733424, 12.760674607101008, 7.938345130796581, 31.13575762275193, 3.694458029411912, 48.75417786313794, 1.757429436918855, -23.910377936456197, 21.844119324171768, 51.524738739852744, 38.016964063168246, 60.5616691931516, 26.27199047288113, 21.510686413296554, 17.154700921326608, 30.332925134201254, 27.342231232163606, 45.28177614923667, 22.116915225428237, 7.453141959589815, 8.114208572100477, -4.580341359907615, 17.783602229620474, -0.0567297233098536, 10.897381691153988, 19.12952856010387, -1.4002882585208738, -9.18870603703378, 11.730505697009248, 25.491581367620636, 9.229621381279722, 7.414159952282015, 7.048396913753095, -4.436328988635218, 0.9856379397344791, 10.23915378847725, 4.109183669289458, 42.016124163132936, 55.50854878870708, 40.50159586055089, 84.92050192589414, 47.722660272545, -39.108069068640106, 94.14874742850442, 97.12527322642819, 64.59723260509264, 77.92756983230991, 34.67077872547193, -35.00038564686949, 59.435459453702364, 27.810512561770757, 27.696261504423152, 24.597863891436063, 16.191523749616277, 16.434005652379096, 16.251228362291556, -1.4470092916392758, -6.807820981198831, 17.23313609527837, 27.17459045553477, 15.998366920801216, 34.04588720808663, 12.812853692097505, 76.65887309463474, 56.20645195523893, 37.79703582008142, 65.18998336355779, 51.75725712443415, 13.892195104008664, 55.33230090073317, 54.08173329842155, 52.54251732604313, 31.325533285346097, 15.430976072705857, 2.7669014323851293, -5.011245656345591, 5.944114762774313, 8.243096367334749, 16.400015588130746, 9.424160799237693, 19.043316574423116, -1.7987099195769254, -0.024711022455818465, 7.483486596346538, 16.52208029738839, 14.232722713373452, 7.3138183339509, 59.8760464756322, 33.640271577803006, 60.077260205678726, 30.47544040412973, 0.7202422361520462, -14.140411755277317, 75.69392795761885, 44.95043789730953, 44.9510239268608, 32.3205035262706, 23.495985940605244, 60.036427104529146, 54.353667128935214, 25.383878863265338, 57.91335526798447, 72.31073649004821, -26.738725512962368, 60.012759185821274, 30.53199492439031, 47.27512787065463, 17.58125379269688, 8.756351614737278, 1.4912993504313288, 0.7803865444325426, -0.6655762371834832, 1.0723978918996206, 1.9514052114174394, -4.1346568361112395, 1.4644368218658677, 5.2046842101369695, -4.708877608835773, 4.637302726898053, -1.924178738342968, 31.810130368930857, 6.025110331441391, 32.986430965573014, 38.46587157805113, 6.161598820644798, 29.65212624609925, 23.524518431697853, 55.56135708856271, 53.54322118139769, 41.823251424192044, 58.00829692319393, 8.089147826777037, -13.900205821468827, 44.64239652776174, 16.912290644739706, 27.582280942214744, -3.0102051484076, 11.294317205025395, -1.7591308424896237, 1.7981321618149249, 8.01233743660623, -0.63590773910407, 14.426603768792642, 50.46149870658108, 33.32747142684738, 65.78449779848714, 22.569761955026905, -27.478815134945677, 19.59036609855136, 52.68232341363446, 37.60924855344096, 15.604224395583074, 6.323819894089909, -0.5838114365476819, 3.649127557775844, -0.010999953185894529, 36.66437609743399, 35.821493987212676, 35.07250309828304, 59.02357386730795, 30.324682549027813, -24.093874606389768, 77.08519142776339, 83.23532917387968, 35.77818173832074, -4.4044568221111575, 65.22278970105597, 30.26153078877083, 42.04511536526688, 7.072949466758018, 5.842236035192645, 29.801036833362712, 15.459040643291559, 14.250334009892454, 6.671966880370303, 4.587141465515315, 2.2583001564250536, -3.0494366205834145, 2.617853080148029, 0.08520000539046829, 1.4863069775730438, 0.1806938021607768, -0.8211345639809078, 18.87088465365304, 10.557023181065958, 14.258362732580004, 18.28990230061076, 3.7631464977283855, -13.411136691002318, 23.865670351855684, 28.734359993938284, 7.230283170913205, 15.661314642081933, -5.4565950230765745, 3.7902361153238715, 2.134455091833335, 5.568144959135699, 7.775781904380718, 5.650357319179651, 0.3491747577830231, 9.241972980588896, -0.16136641727198509, 17.602254818503802, -4.778121832204973, 7.236277621500044, 4.409027202351213, 17.28656480022201, 8.512944204913904, 15.179408380090154, 9.627599877346988, 2.929818167969806, -1.4411498061786658, 9.442034793897768, 1.0697460660842402, 10.052409308165332, 2.983957907784283, 34.856708225466356, 19.62476938036685, 59.27053292467033, -6.567253900430611, 21.405415954084532, 4.44745498349544, 30.057805215141414, 39.81292085723175, 23.733933609887714, 10.569918625924306, 1.8316809843897943, 3.2872446737086225, 54.071443684311895, 37.38159239099255, 81.71289493018406, 34.41140676155446, 23.401323354367605, 35.74540562881364, 72.99093597361664, 74.95402903647124, 83.9308854129533, 13.05943965691904, 2.6345316824455547, 34.91205892292447, 20.273797603839455, 20.488818771635604, -4.441147509349168, 9.494357372154258, 2.2006070826679416, 8.378216493507466, 23.26830036196028, 30.219658264377646, 16.44840393465428, 60.01618023636568, 54.50371891683548, -2.9986077405345526, 71.72306682345092, 121.40479750737657, 36.08742688953561, -76.28773516854204, 80.76509188787686, 42.948841110906905, 29.12244419124259, 13.436010524266916, 1.9102232372163268, 4.795959222110396, -5.428597377293045, 8.100266115808273, -5.155666252433029, 13.563090895512044, 46.961347216638174, 91.55251465373894, 71.24503844934188, 140.72212893485195, -2.5620093628396887, -19.671503022459206, 52.066296272161, 108.78706336959814, 79.73198225234293, 31.607538422843312, 12.234366297528444, 2.6732829467381665, -0.46237146886054437, 1.0299726694240576, -3.0072730970852737, 0.9326611245549447, -1.850338615488982, 5.621350250061769, -5.569294657104442, 4.050659743575237, -4.0279088768440525, 3.7895522264974355, -3.110558663601048, 1.0252125628004185, 1.1519672177964284, 9.306880106675997, -0.16767630325076155, 9.85561016575597, -4.702095667961949, -3.617783892936926, 5.282710662150597, 10.271700769006289, -2.2203816554330817, 5.313322771491491, -2.969538158958421, 3.4729076882719823, -6.605655985437618, 4.14358337902802, -2.7006919211122726, 1.735138893753669, -1.635504574192461, 2.3480201016232924, -2.200654920293327, 3.6312841991766636, -1.7509421007308692, 5.8793746492191765, 51.21260644194571, 66.3202448438079, 68.18745516974442, 72.12451855615555, 12.958404063761918, -13.564260356179773, 63.47697907608831, 78.71962770209058, 56.9349094205497, 25.005680581937938, 2.4637648109153467, 0.8338327954572197, -0.2369548243519446, 2.915431542310241, 15.551584354753864, 13.660909299404675, 17.877018569037215, 6.039152151281462, -1.0138663197158166, 8.89649689963253, 34.25361175354402, 22.80253277212353, 36.42649845716956, 0.8675597653573561, -16.89426804732522, 19.126199233315884, 17.346073316071312, 45.68828969937242, 30.7061373740989, 29.092088801283523, 52.89987345525682, 1.5838602487329467, -12.005627283098221, 47.26009261119815, 32.93111964219945, 20.81680121828436, 16.87908046297324, 9.705051872401405, 71.05194439376906, 21.256349806211716, 104.97814443026395, 2.5878982039463025, 30.389067881249332, 27.06165256983793, 92.38117918550535, 59.95796018356863, 47.958324219172034, 56.00404181816687, 50.19383076895758, 37.69801727005461, 102.39033704073475, 25.844482968696326, -39.821926514568645, 79.69343114739122, 35.94611904096479, 8.133759321619952, 36.14179811430073, 22.03460517964289, 5.227757763263131, 5.384747369175224, 1.758214922780984, -3.681253236439444, 3.607183725846733, 2.1933911144916123, -4.805831108555243, 4.864828458158442, -2.035702446332937, 9.64273084295649, 23.687600361225435, 22.02408566505622, 24.592135307833583, 15.361180991960527, -13.01513141096757, 9.079447050807644, 35.818703487645465, 17.606840696503735, 17.69297385948232, 9.04755438997912, 10.402352213224912, 12.438477399777415, 22.130251380859747, 73.88402586718725, 2.252544788890175, 110.75122945907147, -29.88610917951408, 25.86019999156167, 40.52897194245768, 71.97964524376056, 49.65204248714802, 35.6079687369375, 5.65281685214282, -2.2938416004220343, 6.8877850599252195, 9.29374996687732, 11.820380583376465, 26.98552461532928, 16.144093202919024, 33.038662239126154, 8.543791025508995, -18.390953671648177, 21.3572781949627, 22.4201708292367, 20.88210494676044, 7.051286704151512, 1.3912163108822835, 3.693194263881428, 0.8930576817829116, 16.8618746801639, 28.657241772236212, 12.660625893559498, 63.88027619330255, 7.770328030331854, -19.63682180730467, 39.14311786517867, 32.15165027528068, 7.019652083407133, 25.480133286211753, 6.716786391382345, 35.214383063325286, 4.640307531623613, 32.5343440674102, 2.0681584317530426, 14.20823888689796, 18.8076663731222, 38.00235832520856, 20.59614377698689, 1.617003987746763, 17.406871197443646, 29.86234325326896, 23.033399772766003, 19.324091357745907, 15.472303054468178, 1.3753164240261668, 6.5558679314167465, 10.872007224715496, 28.404053359862</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>20.00055902852358</v>
+      </c>
+      <c r="F2" t="n">
+        <v>28.69137933855449</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
Adiciona o kfold para erro da estimacao
</commit_message>
<xml_diff>
--- a/FiltroOtimoContinuo/ErroEstimacao/ErroEstimacao_J7.xlsx
+++ b/FiltroOtimoContinuo/ErroEstimacao/ErroEstimacao_J7.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,10 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Erro_Estimacao_Amplitude</t>
+          <t>Media_Erro_Estimacao</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Media_Erro_Estimacao</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Desvio_Padrao_Erro_Estimacao</t>
         </is>
@@ -467,14 +462,82 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[-0.37769776158504653, -0.35767167319809684, 0.17968945449856066, 0.8145602575006352, 0.27480292169683246, -0.20454695215897858, -0.32913624675390635]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[[ 2.25468611e+00 -2.71947224e-03  2.69593344e-03  1.63439526e-03
+  -2.37154436e-03  3.24993947e-03 -7.93160873e-04]
+ [-2.71947224e-03  2.23669450e+00 -1.02909676e-02 -1.07938160e-03
+   2.95970473e-03 -1.56154308e-03 -6.44842157e-03]
+ [ 2.69593344e-03 -1.02909676e-02  2.25336895e+00 -3.97587385e-03
+   1.32280850e-02 -4.32147783e-03  5.13154529e-03]
+ [ 1.63439526e-03 -1.07938160e-03 -3.97587385e-03  2.24373352e+00
+   1.66203509e-03  6.86263965e-03 -3.07165972e-03]
+ [-2.37154436e-03  2.95970473e-03  1.32280850e-02  1.66203509e-03
+   2.25318809e+00 -8.92843227e-03  8.55517103e-03]
+ [ 3.24993947e-03 -1.56154308e-03 -4.32147783e-03  6.86263965e-03
+  -8.92843227e-03  2.24276400e+00  1.54092827e-02]
+ [-7.93160873e-04 -6.44842157e-03  5.13154529e-03 -3.07165972e-03
+   8.55517103e-03  1.54092827e-02  2.24965761e+00]]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>-1.386345677960707e-06</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.63777058640036</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>[-0.1292648401907958, 0.062036594434520205, -0.9211541043258772, 2.0887490566931946, -1.3205968171419362, 0.5751739744144813, -0.35494386388358695]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[[ 2.67781720e+02  1.90140135e+02  7.51462098e+01  1.95001742e+01
+   3.01585920e+00 -2.25344780e-02  6.95908453e-02]
+ [ 1.90140135e+02  2.65356572e+02  1.89620384e+02  7.56250739e+01
+   2.01850123e+01  4.00657938e+00  3.85390466e-01]
+ [ 7.51462098e+01  1.89620384e+02  2.69577240e+02  1.93649187e+02
+   7.80598255e+01  2.20444875e+01  4.36236362e+00]
+ [ 1.95001742e+01  7.56250739e+01  1.93649187e+02  2.72067652e+02
+   1.92975423e+02  7.69592867e+01  2.06855813e+01]
+ [ 3.01585920e+00  2.01850123e+01  7.80598255e+01  1.92975423e+02
+   2.68862776e+02  1.91584830e+02  7.65595873e+01]
+ [-2.25344780e-02  4.00657938e+00  2.20444875e+01  7.69592867e+01
+   1.91584830e+02  2.67322256e+02  1.89088973e+02]
+ [ 6.95908453e-02  3.85390466e-01  4.36236362e+00  2.06855813e+01
+   7.65595873e+01  1.89088973e+02  2.64532759e+02]]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9.972063529513905</v>
+      </c>
+      <c r="E3" t="n">
+        <v>21.32772072037319</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>20</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>[-0.14339454108469085, 0.11960066703238818, -0.9949803054570084, 2.1723204512071397, -1.4340851491821278, 0.670651331924537, -0.3901124544402377]</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>[[ 5.05233430e+02  3.59521213e+02  1.41835422e+02  3.72691888e+01
    7.31522850e+00  9.03398774e-01 -4.08527618e-02]
@@ -492,28 +555,23 @@
    1.45017509e+02  3.62599296e+02  5.03142586e+02]]</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[10.963804422385438, -6.419417684714378, 8.591147980621551, -6.909173094399636, 6.654634230543489, 0.262950001603334, -2.3177950756164174, 3.7949114617889412, -1.6758122559240234, -0.029768978717908068, 4.014176256208368, -0.9531122546353448, 7.093454556998203, 53.809865849359056, 26.653957798671954, 51.39348811293895, 32.65744510146598, 3.986092007957211, -11.813679641368909, 86.96642169430693, 61.99121724958726, 61.417224694271965, 11.369343236079029, 9.447396359588822, 8.61314094119848, 25.32722868710443, 30.528222848148417, 20.841381471268022, 10.210560744143208, -1.3980847546838024, 3.0695674465896143, -1.7747976561966217, 2.849855725199466, -2.6821364788362145, -1.948949774707485, 4.445174069940222, -5.658129696904189, 8.48745064910769, -10.124341229837459, 7.4579893792946, -2.8412299537658567, 28.456181601917823, 2.1479150205755317, 33.386754324713294, -1.9809703549019524, 26.877139382619774, 16.114128071228883, 51.87593141529892, 45.102299909789245, 91.71878799623234, 11.161513049923286, 133.0313549697823, 27.40504829822924, 27.94219753824035, 19.413164710834977, 98.85967729254322, 58.841096079212846, 23.334583072972336, 27.11674883890105, 7.231341266378159, 10.258779876908426, -1.6383544817196705, 5.483560648565518, -6.949225144983137, 8.812122051453294, 4.144210959939853, -2.9228163298876346, 14.054664552093346, -1.7249108508642053, -5.383841276492426, 4.067849440687723, 13.507613145109124, -6.239086167997154, 11.196909574010197, 20.29758595259385, 45.83399742016664, 7.228271877745925, 77.14311603227831, 8.782752268058772, -56.23847402274225, 51.195354044877654, 36.25364199684658, 25.42629073635089, 4.614173131366974, 4.788709500316826, -6.131101580910678, 4.216078748321351, 1.673180712322694, -3.7319317192988604, 0.2869401106253251, 1.2170301550327969, -3.439595722250816, 5.236145183917018, -2.726723600739994, 0.7471836172418019, -0.35633697779790724, -0.8348389050712577, 11.563735978989609, 8.43116536373828, 10.21139124141288, 20.340191683038455, -8.980877997315247, -1.2877298031584434, 6.787924533090226, 16.11081108233159, 8.223501755668778, 0.25100628214789794, 9.03151345742128, 6.856848348827693, 9.189043765223737, 20.412357633740015, 9.87368589093272, -22.24069357626605, 62.370558334509944, 36.231491249304966, 47.77771314552982, 41.07970174719967, -3.762467673612946, -13.899823846511211, 55.58210719170114, 35.79237150453775, 25.734854746506308, 1.7283701142715777, 4.801524699697631, -3.0125563251688154, -0.3329854163150259, 4.434475812580423, -1.4439573561749208, 8.703206816959497, 20.516922578258086, 5.906729985283036, 51.85206489444627, 36.45584835106372, 44.662513541873935, 55.65374284175736, 68.51504856694851, 5.104824859852869, 97.5284459181121, 73.5537785569966, 50.73627304671919, 2.6719362137107785, 62.085451968506376, 10.530828941196406, 33.03751743589956, 12.513477432249408, 20.226193963860318, 26.211197816677437, 19.233770498037586, 85.33300660636833, 18.2933030828992, 45.451180474899104, 0.671116113184155, 52.57744695599746, 22.740238178649587, 49.63775479007014, 47.3898186327428, 36.65153764112745, 37.979384947799694, 13.109728578987514, 38.257537678349536, 1.5953853616442046, -14.660526752895265, 66.48422293440566, 34.95657838786495, 34.43649749190274, 61.4841918448967, 68.36359935155949, 12.720756360771759, 134.96793979080866, 48.82213073925834, -50.428727803547105, 108.70884680164113, 38.73886873340189, 34.06583296633009, 24.597870065515718, 23.642155689697226, 11.227681205848034, 14.480429579338235, -2.3730794373736224, 5.53713319237124, 9.62323198415842, -3.9005252955596346, 2.8127587802556278, -6.89976918044721, 11.784067461410968, -3.027320327842644, 6.339343088582748, 23.758778625798474, 2.725419172498185, 28.42679655385639, -6.642065378407965, 4.5081557348771355, 6.51810031100843, 20.862940886987168, 14.352708767816798, 7.957536399803486, 1.763030785883009, -3.611079014369215, 9.275054100954812, 0.8032161810131715, 10.864302880382471, 10.20677393076912, 49.111447993594545, 37.3803474218615, 3.164461246587912, 81.80963387984023, 26.01106671046489, -54.786040580160325, 60.841619613837494, 30.428102622828405, 29.214102009818433, 14.372792887768673, 1.9236117359083167, 22.51002096123455, -5.6537346367639945, -0.8064812234167817, 5.1214371384684485, 7.672238602637837, 11.560652172435788, 2.6746901454245195, 0.16811660915466708, 5.46471290261834, 1.6858156400159823, 0.4288935179988598, 4.349143124932903, -4.8497480847844, 5.107480622743742, 3.827691185073015, 3.864022930698831, 1.7303702624289046, 2.7816986253773437, 1.7622950886711932, 0.9154552685812831, -2.6956466942265136, 1.9077778718086607, 2.8922364505300115, 1.9971651505634354, 1.5894752422200473, 14.12772872945139, 0.14220393286140975, 24.063877286073797, -7.6034401507461205, 13.67269665423968, 0.5119917134309315, 12.765007901164953, 8.305583869982264, 47.455628712492356, 22.69594376558142, 35.717158013867966, 26.449702100859184, 0.32679382525449796, -14.342018235891063, 44.26309187426695, 27.269380666876728, 18.92661740337368, 6.5904982134509, -1.942846485640219, 5.2978896246523846, 26.592667837472824, 18.122784342488572, 26.61161192944742, 22.87348069014812, 29.50555635971878, 13.991792584531545, 64.70106156297116, 62.4952942792778, -5.7429396318964905, 19.95763544769794, 29.646249659004283, 41.09474068066718, 24.92590090935548, 9.090439126403512, 9.969289584845132, 4.111122531819541, 21.643070320056726, -4.564298110319754, 26.159065590953563, 12.22646466425677, 20.641584570725982, 39.19203245692782, 13.01443498809456, 14.332250716611682, 3.5725477942432264, 44.16978156079248, 39.10987424348361, 17.50803219753817, 44.82933776563355, 9.381375446574694, -37.81055168109461, 36.069606458521115, 7.480051561439793, 22.674391953409554, -3.4254575465872357, 6.7797013998456555, -1.339268288830581, -2.030867217461452, 7.941542608092689, -13.50057476111568, 9.925101253132055, 1.7699695493157392, 18.632801274711113, 2.6255934973794197, 24.48206139124677, 2.889902768331595, -22.73610868080233, 25.546249644461184, 9.944702647763862, 17.93404062627791, 7.322012451263397, 19.831283322910842, 51.53835767337931, 14.881030571421562, 66.17775624563444, -8.726691356930354, 26.29572142072027, 16.01075050272229, 58.66326255545397, 36.521781330232265, 27.306187925251752, 27.779316302747702, 10.223999069751343, 29.062581476765708, -2.2058410822553967, -3.4011319345563606, 20.592567103897732, 17.367627671341747, 14.27872314897354, 9.381297993811822, -1.8555961246797155, 1.212212324974744, -0.18376428570115602, 1.2522895030552288, -3.029845853588345, 4.618541348781362, 18.54151005321054, 38.92740179276902, 25.3868076120717, 55.67275137323004, 14.258622151404339, -15.611362023552203, 34.89151751140287, 56.451292542961895, 57.01302809495756, 14.311724909377462, 2.1675148696117077, 3.0636097837153784, 29.121419313641276, 14.374953197742647, 31.9358115547629, 32.66001453974671, 9.403567526705494, 61.150499280172184, 4.701128658043899, -48.97986299924297, 45.82242525035449, 27.09774706853283, 15.057403491709286, 10.963486276871636, -3.841606962764413, 3.300642101360493, -0.9812985578081236, -1.9386700837531026, 1.5062811466568613, 4.318209413802614, 9.489993676296358, 14.264017129042365, 26.205408731762304, 21.18373190421681, 17.410472521219603, -19.85809410459829, 27.102376255896814, 25.86063759110166, 18.609492222317357, 43.451259461102964, 20.72249610425556, 16.235047370378147, 47.02050550851601, 8.342255917540342, -30.76337992519582, 41.263987126914564, 21.70091225107124, 42.42181796268072, 28.561534569973446, 24.858494627954002, 30.926734941137198, 0.8130217980017278, -18.91598511788269, 48.08167568506626, 51.714072243114124, 32.04211352896489, 36.47068295764774, -6.188925082967806, 4.691521740657464, 35.31951688104043, 45.03630853570855, 42.87085869824372, 16.397498805789027, 4.946714936871729, -4.514589879289554, 33.30150219693623, 14.612217262830415, 18.425109179406196, 16.854963566938622, 7.326099128849769, 17.421160093010258, 18.173884575885047, -2.783647168005004, -11.446108290072482, 24.228234091954267, 11.133028841824366, 31.859562417846213, 8.329491705456217, 31.102755417530652, -2.7124313338280004, 4.340950314098947, 4.115427660831929, 21.111264105042434, 16.29684613313592, 8.594879358757913, 4.7723524280366, 1.0960914346803592, 0.6307536665499364, 14.563679985686496, 7.6856163317956785, 14.166667443780295, 14.946205631332814, 0.18711464265571465, -8.996668696445509, 15.312197031972842, 30.02289785122899, 11.120740665612534, 27.198743940369926, 14.069593592029403, 11.399682516770994, 1.5895364751222898, 20.313552641793386, 2.3861631733468935, 19.119742723194296, 12.78668072308835, 4.512044134011193, -1.0509962779359379, 4.867827822838006, 0.7977792968374384, 16.1083911145095, 8.086329875656576, 10.581826120831554, 4.459924834969229, -11.374138399571741, 20.060896043754255, 3.8793189344019323, 7.476330353704768, 7.7675561705809075, -6.311219759104397, 8.177891510411236, -8.700401307650782, 7.185932653436935, -6.967029832405512, 7.19499932160935, 16.816910188496138, 9.797774531589688, 30.031230551656606, -3.2057851528208836, 4.1232926191771355, -1.880598105784996, 27.292589032259293, 12.569544896069628, 7.106430360878286, 5.916512340105086, 4.20236578205249, 62.33133314943409, 24.876747775558243, 98.6698572986256, -4.575486128171008, 32.57203156758396, 50.96485566408073, 64.72139254237442, 45.65309471828126, 55.57142083096507, 71.37510409999456, 32.47352476653593, 85.1955438011851, -34.30211604321703, 21.512767226466593, 48.95341035886932, 69.40768813059566, 70.33743675811593, 44.17444935613969, 1.5516421440417787, -12.731200262664107, 39.33586263105635, 36.467673635472856, 19.927290880127302, 10.10061885720237, 15.967142024803163, -0.9176835209061842, 4.785454586738169, 24.493384706251938, 11.39052641833576, 49.270464824631276, -5.852269263876553, 7.108178018505612, 4.522845043055673, 26.705186805197673, 11.719271188538729, 13.922920993416463, -0.3619554078176276, 3.794967038919492, -2.09594482148852, 0.038212215764959756, 0.7543538390741511, -3.721932903575941, 2.259223920031712, -1.3657481808214091, 5.311392578220338, -0.9563789954061519, -3.383591915898333, -1.4092593992358826, 2.183050112005874, 0.39775715801125244, -0.364427456677652, -0.23373924457681666, 0.9507203273638245, -3.4917064030092178, 2.056750722164607, 2.127247068810753, -1.7500820142228632, 3.061090970143044, -2.560772896933708, -0.5498679837659437, -0.5018550718716269, 0.7194361617006007, 0.18572509208188853, 3.9256757833546114, -5.268733106220703, 3.8296236803907524, -3.186283791111265, 47.92493611795526, 14.390824814891161, 57.18673126386305, 2.36198708940503, 3.4000219800295213, 2.278374976924689, 52.51206325430047, 36.881433036051384, 37.54310961745041, 11.686942417478768, 39.05125208148441, 10.737190277553324, 5.22518932536504, 18.950382225796545, 15.5780513906587, 12.524108107721403, 29.986620808347496, 15.66656466450523, 19.51906952400509, 3.5069212191571992, -0.4757855675860867, 16.339303066191484, 10.965097279066942, 11.49347498978327, -12.716992329905972, 9.969963353292963, 2.9214365857395337, 27.24583566369341, 25.90330038063462, 10.959796244776548, 52.867878039638484, 10.901475625110976, -41.732740084148475, 37.60899443815548, 24.54104491332751, 12.76127706542887, 14.27522726239414, -3.2098397333417488, 3.129460251496576, 0.1895534365347641, -0.8376076255928464, -2.462461138847518, 4.369994230515522, -5.459570012147273, 5.71693745132891, -6.259833151006488, 7.475119153676498, -6.7403976673748405, 4.851161325616529, -2.257730570446203, -2.479309512502845, 16.27965170871085, 2.901442530659949, 12.182093116463511, 12.525761171412885, -2.897325082659222, -6.955689966885845, 17.306880696437773, 5.649888189046847, 9.257683080878788, 2.1893780405379877, 1.5273751315339368, -1.310698509917214, -0.25141499417080093, 0.6502444259078368, 3.7870988453115992, 3.5652523532208678, -0.5729916594838279, 0.35714584649748815, 0.4541811290783624, 7.511882672059571, -4.849462957315222, 19.344810784318987, 3.423564401903633, 74.98481927818568, 89.14330945590538, 26.781905194418428, 132.5068212423966, 39.74379119373174, -109.88155380612822, 118.2481702285384, 67.55819356372366, 50.5207080515278, 33.58246450166527, 21.080671105101707, 16.56595412364965, 27.675908526273606, -3.2446853356833856, -3.9077179371201614, 30.818362045655245, 18.059155420960607, 24.838896306893314, 27.130733500179687, 1.1718980105541021, 36.33779899500191, -3.959806388455533, -14.981409516980822, 83.04345760058146, 34.829640340708565, 85.27128054006693, -6.621536296108122, 3.129578581665214, 16.459954889265614, 63.99621114141256, 40.095735825406784, 27.35293134073448, 11.434376719240841, 0.1664410395961866, 8.752137671236818, 4.660636378766872, 1.6752812508682133, 45.5622847967967, 18.168286504204502, 71.85930317786386, 1.871193364827171, 22.581979688156537, 6.277564022456815, 57.17968529881715, 38.98876576160699, 32.92460729893822, 54.49298216248907, 43.84990721853758, 126.04935821267863, 41.664081563767866, 142.08667202253656, 58.36616538913404, -39.75914258572652, 88.40945079905359, 148.7813657104155, 85.74457806944847, 28.87125846121046, 48.14151308502555, 40.712025156362586, -10.085872142719888, 38.049418492454976, 17.049044310239246, 24.757711725775835, 2.5569053420625387, 21.89464402795654, 1.2175054263138243, 14.746715891822127, -2.865212998948401, -0.7737702481971208, 16.456341858326322, 7.959308532120553, 12.957680245401498, 2.9725822671041495, 4.5218664339816605, -4.935067125612017, 2.2131240325296915, 3.6245355603642193, 1.3804583531960533, 24.496380141047677, 6.786818031962795, 30.11055239010064, -16.295869452957117, 11.166858697453705, 3.110660150521165, 27.407502081054353, 10.59282077863541, 7.393185437824538, 5.507318359147138, 8.042877599767003, 18.85125663903551, 28.370644071068178, 58.73552768045741, 86.97037306782097, 64.30077955005399, 119.04395421576336, 88.01018237952611, 79.91735362287329, 62.02043045737385, 149.8166989125922, 103.6966646773953, 77.70077482884722, -16.774142332553993, 90.0001007452624, 43.620969733449726, 31.09011966476024, 7.050925866751468, 10.27279809445509, 1.0341878690208806, 1.8413396425912634, -7.808699023649386, 13.48723037287959, -8.746408136188661, 9.146486750798845, -5.8782991632518655, 2.245984260020897, 3.3726576826912176, 0.748718881086484, 5.890697553204161, 10.411016195297712, 2.7601259770211364, 1.0762397988680803, -2.8373011882814874, 9.394875088170483, 2.2640258039997105, 8.255417114722412, -5.51876443012742, 7.480362062042602, -7.266961622773849, 9.186070732971494, -11.036386763269944, 8.2739376392174, -3.426411656753448, 1.6347063877521584, 30.558507958212818, 6.056996331385591, 32.50688369480063, 8.045485297318955, 1.2061224922382792, -8.24653392335716, 38.170339729711806, 14.069973250111007, 14.53515590440337, 6.0167530188606015, 43.206175742087005, 34.41234056600142, 37.561419003521216, 51.38165981121489, 5.871981738685577, -43.92262693537896, 72.50348770547032, 33.54159230109732, 30.8326839443879, 8.05989147559968, 2.60969934610743, 26.68877652808804, 11.135594687586135, 29.24222332181554, 14.379621426103682, -2.6603064577872786, -3.076542350633499, 25.9568801029108, 24.083485377784406, 37.40222329671735, 42.09664524782929, 37.04475182550744, 24.141147659240126, 22.415090713392743, 41.40443363472719, 70.8848647443081, 96.37217794447824, 63.81005469959287, -28.091418952441444, 14.713500450022973, 58.348359696537436, 46.376366816073, 29.562994724754226, 15.704569614645688, 23.375071559066097, 12.081660348973386, -1.4230330734703145, 37.517175244411106, 15.805617261165844, 0.5504919767299157, 24.602959543871734, 12.465540852789625, 20.902218287111566, 6.9160621698991935, 2.5991523980431452, -2.0082119480369442, 10.321064592332476, 15.338806685650274, 18.45862196628877, 6.821344339056253, 21.334664381908354, 4.677385872848092, -17.422818727325687, 26.740671598077153, 13.122260728249438, 17.757261979892956, -3.3172038586451422, 13.59330269902419, -12.909784764611548, 16.25724252218062, 3.06806234192549, 2.3215871668116383, -0.18542607949998002, 3.6354894413559293, 54.10550566812083, 61.991470144663595, 32.26556657417687, 122.92062176129146, 30.369965150339226, -98.83442911983367, 101.0378553583163, 70.12373319138246, 34.04583775842246, 12.128679863370477, 12.613450152062498, 6.82980414403246, 8.286031306165425, 6.781535908516424, 34.09516254675364, 40.86478719022034, 12.092013018864272, 65.88195537076346, 4.683202260255598, -8.060493474319646, 56.53340948773249, 62.99678291216307, 41.81712043979095, 28.936226362819582, 78.89283808861954, 83.70874131381474, 44.66326407890307, 92.38777683477234, 44.608673013745715, -22.58546857944628, 83.13056387805715, 37.65904820812647, 45.15834236878267, 33.77396072796406, 19.96137695138697, 22.030273680579263, 11.015547734156767, 7.026780337493264, 4.5518706912210325, 27.537472528181894, 12.237832532110492, 20.70867170300941, -1.510347341614737, 10.778225686203191, 1.7083804020953186, -0.01869015171678895, 0.12935111754559148, 1.108195122777898, 0.8759070893103593, -2.9213331837764165, 1.800146319868821, 6.657890902693673, 21.535511679424964, 1.3918333918494241, 29.310315296108456, 11.592626745703896, -29.987926738694284, 19.720948415139013, 10.075924427262445, 16.95577453610666, -2.961307190545028, 1.603887634048637, 6.172151771516482, -7.571419001200001, 8.643923712403197, 11.64885759750716, 31.476473262337457, 1.5588952798263165, 94.74111457123448, 67.21170103657474, 23.514627414497255, 133.17948651711828, 36.46734109297586, 10.516684614782037, 76.11962348451203, 70.10006646215412, 83.75746776103622, 59.6371345944251, 27.689873853910157, 32.132216432460474, 51.51389906889004, 24.880556919001535, 29.072953722163394, 26.228496994206125, 25.38871828986724, 40.234563980622816, 17.601731490070513, 6.853632712315957, 15.552379085911378, 15.086737955318773, -3.7949097537349252, 5.807741969498272, 2.6092444141494253, -2.5236650273872767, -0.313652376709598, 1.6217185830434797, -2.998734187671086, 5.63992475272879, -1.0724448868000873, -1.3151340588921898, -1.0362558361752228, 0.8267726482017168, 2.4346809754984244, 2.9284784271776996, -4.476455721668018, 5.14196410041807, -5.848238782953469, 20.2472427193008, 7.503363490580735, 43.4332945674136, 41.67058425375028, 35.56174728486343, 35.17944140867541, 37.784325368749876, 0.3188567949374175, 46.00617063276987, 69.40439002678448, 46.62247943554402, 41.26052552633463, 16.58303243169192, -22.684945852814934, 42.2955477129314, 12.33191029785181, 19.75162958413654, -3.4470384410390817, 8.294147140903513, 7.747935142231952, 6.552130642489152, 6.432672373121916, 1.8346242796124343, 2.799378273187912, 1.0551115370000375, -3.7256796723599277, 9.600394337437052, -0.980788974568144, 2.75530549353078, 5.287242036656306, -2.334154124797226, 5.881121098230103, 46.50222926692312, 12.958987865231421, 69.84134752324636, -12.469918320086045, 14.224445483350564, 8.164558324811061, 84.3475879143082, 38.3893166649647, 95.65470120416634, 2.1832530007062303, 73.86242486016297, -16.181083886300577, 39.32713504495533, 27.85352959879806, 48.565184725666654, 29.623747033926584, 33.08370384301778, 8.10345594495031, 12.679402558588482, 7.193041917390195, 4.351938047528677, 7.168231722846757, 17.117574596608396, 7.216575781077054, 2.831210427315554, 6.731950130052189, 6.800909117516573, -0.6487533213572941, 8.199956212972227, -5.000564494756847, 11.446129209292348, -5.741231434894834, 27.50083823117454, -0.03256431681068861, 16.56513004497762, -0.19537019931522526, 2.603253895291843, 9.035976297124169, 12.635875005705671, 14.418750173000687, 1.965008885765979, 0.15283054202871843, 4.502758034331163, 6.454043093352853, 7.963742350028338, 8.027052600914764, 10.967112294295905, -1.2430798571267325, 9.637785107184861, -4.185444591588373, 14.057581237090247, 4.205307322509485, 7.017243538340267, -2.728310162701156, 22.88486646364003, 62.445787169865454, 14.92846924337293, 100.99620624453172, -21.01775646758702, -11.15044046930089, 29.60692127146112, 79.1522449103986, 30.667134507660307, 33.2085825845372, 4.428035421125756, 8.34579839721005, -13.594798608401991, 11.870630835089448, 10.524744505153002, 12.85607548333148, 27.456035792398005, 22.058636447703805, 25.369478407887996, 31.83273816191705, 51.6239107853566, 96.67256936560901, 81.96836966182568, 38.000780842805796, 45.17462656350512, 81.02807589701786, -12.68394152521525, 81.59382369416979, 34.892024252939095, 21.381873093746858, 26.6898730927101, 43.88052032002462, 58.69283858569574, 54.49221359105495, 90.70663429834136, 8.057738525756491, -11.309313322303531, 149.9696988347689, 82.04954840310013, 70.69321799755184, 48.07921836861895, 51.25486691648695, 4.789788441271174, 76.83929269147256, 39.07468499703156, 16.654586750826763, 9.168238978750626, 13.28828219434635, 6.255172248358738, 2.3983693174398235, 0.6226764643217437, 5.010000035402371, -6.603243649643, 8.847824134689734, -2.876810983999812, 0.7289842837420277, -3.279758008755326, 5.220328211977897, 6.045818164917872, 0.8467414303055651, 10.281245726770265, 14.548947996130225, 20.65414895337922, 10.85002491779273, 48.14222919523364, 37.333154111143884, -11.923592311347413, 84.34912259516973, 36.48971880613473, 6.629687128247255, 102.3591405134866, 48.34000550201765, 101.42158253113894, 11.900038937739112, -55.164177107977885, 82.97776500627177, 42.62997530828501, 32.25884538887614, 10.089739839053118, 2.9171849752851178, -1.5054024057408553, 0.9810516970075019, 0.17783921474722353, 2.455688890263451, 2.5209650809638458, 43.67136869689038, 55.41437235759426, 22.932818553781573, 96.35868371238821, 9.747147943375012, -73.1014150786105, 90.85902103779652, 48.625433657605825, 45.742383021999984, 21.96689301306667, 17.178526830136214, 33.4189997729633, 17.83360055052242, -1.2012282113697452, 137.6529493657726, 78.18520718641314, 93.74203968862375, 137.18966810076998, 48.844121850945385, -6.68759587158339, 140.49399980921865, 61.815555091854705, 92.70675957628053, 35.99511904554866, 56.14541511011397, 39.81933510932956, 23.032971849978793, 38.484868807966265, 10.591570008600257, -21.053853002964225, 54.317726981909914, 17.736994007508446, 10.24222477852025, 14.353666201526924, 2.6522529282787515, 7.7936898510074935, 24.295435810543896, 26.765346672818794, 21.000931483121946, 50.10486183278114, -11.208611569072204, -10.404789846072106, 32.854852725233535, 34.53332998120255, 20.54591174808724, 15.048224903140508, -5.719938754180203, 8.648548614259598, 6.704276487626362, 11.747295787191081, 7.869879894559801, 18.43688919209728, 0.481985055793956, -14.613247780029923, 20.571616697026695, 8.738871127355821, 5.450928259405285, 4.454183167999255, -1.8926422365657665, 35.211512271180766, 16.134215741640418, 34.689377645757965, 17.31862858438992, 5.757139426675138, 7.936813467215693, 60.549662952987575, 59.97838400928519, 46.785473248181134, -5.759589951209215, 26.451987729513107, 11.585024235400546, 39.45981654852574, 54.55049304579518, 42.50165691823445, 53.50420620296736, 36.54001488731066, -14.457335163962142, 22.99693410426017, 15.874055394573483, 43.86531070314011, 18.998111027559478, 10.216708714382515, -2.1688154630695147, 9.30722706654009, -6.86186042810584, 4.194115990233447, 2.4104280459755283, 5.949323180192973, 1.7396956994814392, 12.342563462758726, -6.853514567646357, 5.794459899484764, -4.276905120697153, 16.7451891751795, -3.1887387927617126, 4.931128976121094, -4.047461569276654, 1.2256132895263046, 1.3845217294259675, -2.4414264424521335, 4.031243450889584, -5.647855401984925, 2.705870975747417, -0.927362293507838, -1.3579713026872344, 4.83524709778491, -3.706493353178872, 5.662867262929591, -3.8645897750975413, -4.277185248832327, 5.256281878860347, -1.3792776923857717, -1.5153871093967497, 20.43606059806084, 2.1423425907507117, 17.261314320142652, 14.343504929507482, 37.501092170756706, 43.42733246372812, 33.239205758811735, 110.4293122212254, 18.38992259318576, -73.81680759690288, 94.61169623650461, 38.88785958826219, 61.8586380765901, -1.7725944891724055, 13.985122702558229, -1.3917958749710468, 27.50634331359692, 7.073048414733424, 12.760674607101008, 7.938345130796581, 31.13575762275193, 3.694458029411912, 48.75417786313794, 1.757429436918855, -23.910377936456197, 21.844119324171768, 51.524738739852744, 38.016964063168246, 60.5616691931516, 26.27199047288113, 21.510686413296554, 17.154700921326608, 30.332925134201254, 27.342231232163606, 45.28177614923667, 22.116915225428237, 7.453141959589815, 8.114208572100477, -4.580341359907615, 17.783602229620474, -0.0567297233098536, 10.897381691153988, 19.12952856010387, -1.4002882585208738, -9.18870603703378, 11.730505697009248, 25.491581367620636, 9.229621381279722, 7.414159952282015, 7.048396913753095, -4.436328988635218, 0.9856379397344791, 10.23915378847725, 4.109183669289458, 42.016124163132936, 55.50854878870708, 40.50159586055089, 84.92050192589414, 47.722660272545, -39.108069068640106, 94.14874742850442, 97.12527322642819, 64.59723260509264, 77.92756983230991, 34.67077872547193, -35.00038564686949, 59.435459453702364, 27.810512561770757, 27.696261504423152, 24.597863891436063, 16.191523749616277, 16.434005652379096, 16.251228362291556, -1.4470092916392758, -6.807820981198831, 17.23313609527837, 27.17459045553477, 15.998366920801216, 34.04588720808663, 12.812853692097505, 76.65887309463474, 56.20645195523893, 37.79703582008142, 65.18998336355779, 51.75725712443415, 13.892195104008664, 55.33230090073317, 54.08173329842155, 52.54251732604313, 31.325533285346097, 15.430976072705857, 2.7669014323851293, -5.011245656345591, 5.944114762774313, 8.243096367334749, 16.400015588130746, 9.424160799237693, 19.043316574423116, -1.7987099195769254, -0.024711022455818465, 7.483486596346538, 16.52208029738839, 14.232722713373452, 7.3138183339509, 59.8760464756322, 33.640271577803006, 60.077260205678726, 30.47544040412973, 0.7202422361520462, -14.140411755277317, 75.69392795761885, 44.95043789730953, 44.9510239268608, 32.3205035262706, 23.495985940605244, 60.036427104529146, 54.353667128935214, 25.383878863265338, 57.91335526798447, 72.31073649004821, -26.738725512962368, 60.012759185821274, 30.53199492439031, 47.27512787065463, 17.58125379269688, 8.756351614737278, 1.4912993504313288, 0.7803865444325426, -0.6655762371834832, 1.0723978918996206, 1.9514052114174394, -4.1346568361112395, 1.4644368218658677, 5.2046842101369695, -4.708877608835773, 4.637302726898053, -1.924178738342968, 31.810130368930857, 6.025110331441391, 32.986430965573014, 38.46587157805113, 6.161598820644798, 29.65212624609925, 23.524518431697853, 55.56135708856271, 53.54322118139769, 41.823251424192044, 58.00829692319393, 8.089147826777037, -13.900205821468827, 44.64239652776174, 16.912290644739706, 27.582280942214744, -3.0102051484076, 11.294317205025395, -1.7591308424896237, 1.7981321618149249, 8.01233743660623, -0.63590773910407, 14.426603768792642, 50.46149870658108, 33.32747142684738, 65.78449779848714, 22.569761955026905, -27.478815134945677, 19.59036609855136, 52.68232341363446, 37.60924855344096, 15.604224395583074, 6.323819894089909, -0.5838114365476819, 3.649127557775844, -0.010999953185894529, 36.66437609743399, 35.821493987212676, 35.07250309828304, 59.02357386730795, 30.324682549027813, -24.093874606389768, 77.08519142776339, 83.23532917387968, 35.77818173832074, -4.4044568221111575, 65.22278970105597, 30.26153078877083, 42.04511536526688, 7.072949466758018, 5.842236035192645, 29.801036833362712, 15.459040643291559, 14.250334009892454, 6.671966880370303, 4.587141465515315, 2.2583001564250536, -3.0494366205834145, 2.617853080148029, 0.08520000539046829, 1.4863069775730438, 0.1806938021607768, -0.8211345639809078, 18.87088465365304, 10.557023181065958, 14.258362732580004, 18.28990230061076, 3.7631464977283855, -13.411136691002318, 23.865670351855684, 28.734359993938284, 7.230283170913205, 15.661314642081933, -5.4565950230765745, 3.7902361153238715, 2.134455091833335, 5.568144959135699, 7.775781904380718, 5.650357319179651, 0.3491747577830231, 9.241972980588896, -0.16136641727198509, 17.602254818503802, -4.778121832204973, 7.236277621500044, 4.409027202351213, 17.28656480022201, 8.512944204913904, 15.179408380090154, 9.627599877346988, 2.929818167969806, -1.4411498061786658, 9.442034793897768, 1.0697460660842402, 10.052409308165332, 2.983957907784283, 34.856708225466356, 19.62476938036685, 59.27053292467033, -6.567253900430611, 21.405415954084532, 4.44745498349544, 30.057805215141414, 39.81292085723175, 23.733933609887714, 10.569918625924306, 1.8316809843897943, 3.2872446737086225, 54.071443684311895, 37.38159239099255, 81.71289493018406, 34.41140676155446, 23.401323354367605, 35.74540562881364, 72.99093597361664, 74.95402903647124, 83.9308854129533, 13.05943965691904, 2.6345316824455547, 34.91205892292447, 20.273797603839455, 20.488818771635604, -4.441147509349168, 9.494357372154258, 2.2006070826679416, 8.378216493507466, 23.26830036196028, 30.219658264377646, 16.44840393465428, 60.01618023636568, 54.50371891683548, -2.9986077405345526, 71.72306682345092, 121.40479750737657, 36.08742688953561, -76.28773516854204, 80.76509188787686, 42.948841110906905, 29.12244419124259, 13.436010524266916, 1.9102232372163268, 4.795959222110396, -5.428597377293045, 8.100266115808273, -5.155666252433029, 13.563090895512044, 46.961347216638174, 91.55251465373894, 71.24503844934188, 140.72212893485195, -2.5620093628396887, -19.671503022459206, 52.066296272161, 108.78706336959814, 79.73198225234293, 31.607538422843312, 12.234366297528444, 2.6732829467381665, -0.46237146886054437, 1.0299726694240576, -3.0072730970852737, 0.9326611245549447, -1.850338615488982, 5.621350250061769, -5.569294657104442, 4.050659743575237, -4.0279088768440525, 3.7895522264974355, -3.110558663601048, 1.0252125628004185, 1.1519672177964284, 9.306880106675997, -0.16767630325076155, 9.85561016575597, -4.702095667961949, -3.617783892936926, 5.282710662150597, 10.271700769006289, -2.2203816554330817, 5.313322771491491, -2.969538158958421, 3.4729076882719823, -6.605655985437618, 4.14358337902802, -2.7006919211122726, 1.735138893753669, -1.635504574192461, 2.3480201016232924, -2.200654920293327, 3.6312841991766636, -1.7509421007308692, 5.8793746492191765, 51.21260644194571, 66.3202448438079, 68.18745516974442, 72.12451855615555, 12.958404063761918, -13.564260356179773, 63.47697907608831, 78.71962770209058, 56.9349094205497, 25.005680581937938, 2.4637648109153467, 0.8338327954572197, -0.2369548243519446, 2.915431542310241, 15.551584354753864, 13.660909299404675, 17.877018569037215, 6.039152151281462, -1.0138663197158166, 8.89649689963253, 34.25361175354402, 22.80253277212353, 36.42649845716956, 0.8675597653573561, -16.89426804732522, 19.126199233315884, 17.346073316071312, 45.68828969937242, 30.7061373740989, 29.092088801283523, 52.89987345525682, 1.5838602487329467, -12.005627283098221, 47.26009261119815, 32.93111964219945, 20.81680121828436, 16.87908046297324, 9.705051872401405, 71.05194439376906, 21.256349806211716, 104.97814443026395, 2.5878982039463025, 30.389067881249332, 27.06165256983793, 92.38117918550535, 59.95796018356863, 47.958324219172034, 56.00404181816687, 50.19383076895758, 37.69801727005461, 102.39033704073475, 25.844482968696326, -39.821926514568645, 79.69343114739122, 35.94611904096479, 8.133759321619952, 36.14179811430073, 22.03460517964289, 5.227757763263131, 5.384747369175224, 1.758214922780984, -3.681253236439444, 3.607183725846733, 2.1933911144916123, -4.805831108555243, 4.864828458158442, -2.035702446332937, 9.64273084295649, 23.687600361225435, 22.02408566505622, 24.592135307833583, 15.361180991960527, -13.01513141096757, 9.079447050807644, 35.818703487645465, 17.606840696503735, 17.69297385948232, 9.04755438997912, 10.402352213224912, 12.438477399777415, 22.130251380859747, 73.88402586718725, 2.252544788890175, 110.75122945907147, -29.88610917951408, 25.86019999156167, 40.52897194245768, 71.97964524376056, 49.65204248714802, 35.6079687369375, 5.65281685214282, -2.2938416004220343, 6.8877850599252195, 9.29374996687732, 11.820380583376465, 26.98552461532928, 16.144093202919024, 33.038662239126154, 8.543791025508995, -18.390953671648177, 21.3572781949627, 22.4201708292367, 20.88210494676044, 7.051286704151512, 1.3912163108822835, 3.693194263881428, 0.8930576817829116, 16.8618746801639, 28.657241772236212, 12.660625893559498, 63.88027619330255, 7.770328030331854, -19.63682180730467, 39.14311786517867, 32.15165027528068, 7.019652083407133, 25.480133286211753, 6.716786391382345, 35.214383063325286, 4.640307531623613, 32.5343440674102, 2.0681584317530426, 14.20823888689796, 18.8076663731222, 38.00235832520856, 20.59614377698689, 1.617003987746763, 17.406871197443646, 29.86234325326896, 23.033399772766003, 19.324091357745907, 15.472303054468178, 1.3753164240261668, 6.5558679314167465, 10.872007224715496, 28.404053359862</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="D4" t="n">
         <v>20.00055902852358</v>
       </c>
-      <c r="F2" t="n">
+      <c r="E4" t="n">
         <v>28.69137933855449</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="5">
+      <c r="A5" t="n">
         <v>30</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>[-0.15107749697392545, 0.14395420064686185, -1.0199135124499774, 2.19982973068618, -1.4696038891478476, 0.6956192782245417, -0.39880831098583314]</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>[[ 7.07173395e+02  5.10835430e+02  2.03794986e+02  5.18478822e+01
    7.51210301e+00 -4.07658239e-01 -3.65252170e-02]
@@ -531,16 +589,249 @@
    1.97562541e+02  5.03460624e+02  7.07724279e+02]]</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>[-9.2655252346655, 18.969115709766967, -4.069553898652471, 9.097430361544504, -1.8880121098669242, 3.6947268176070516, -1.719129932428386, 11.510412664680677, -1.866999363495534, 6.160550678898808, 0.240807224484465, 52.366298527581286, 20.785834737888067, 49.34317350589857, 37.05304084076107, 26.6300919608355, -10.481134354084922, 108.03968936569116, 31.99009890412182, 68.19498042881474, 29.73338112140445, 53.21235616735298, 39.66464158305787, 49.05644709830774, 28.231160860141088, 70.83397729374367, 96.26163330559328, 16.693442119124285, 137.3397419019256, 16.310159704521954, 23.814816813062635, 9.253674868921197, 85.51953891071415, 59.6347546632478, 29.939080451139755, 13.452864176847017, -2.042698636002616, 12.280993759213803, 13.499899573728907, 0.18499706351561152, 17.003642782628447, 0.44798973219202765, -2.7346195559895, 23.6964491929645, 39.24366424202003, 61.85419292463425, 13.93032448343105, 91.4518718011737, 32.133114388414896, -46.19003092654687, 58.369353841579326, 51.2461711604376, 104.3274510721532, 42.78078060655608, 27.632915803721033, 50.32432660490427, 15.90605352400965, -13.316642855602439, 62.48168278930341, 36.42909823565601, 25.28190591445421, 7.548499408908256, -0.7456957861852005, 7.51052794147119, 17.320589642715483, 8.0292379076627, 24.84562177055678, -0.18571677680105392, 6.349193619389467, 27.936640322152275, 58.988934508774136, 32.87715727130691, 60.90837936327695, 5.119166827542443, -21.40033664568029, 57.51543240277963, 51.3840093149429, 14.245970215079097, 13.292704059481075, 31.76129931898155, 37.94107832435876, 34.54812910870922, 39.06022447578209, 4.28849075915025, -19.03239354249989, 40.9052590408335, 26.637340424291196, 15.07170134997686, 1.851437484565967, 6.211122206181658, -2.6977880211973497, -1.6661953132984293, 5.247428697555469, -2.6750139815619156, 9.27251302715532, 10.447990424789324, 5.404168032785, 26.53852524392566, 17.317403971444286, -8.551139269867718, 44.45834950418678, 15.277921001711604, -7.9223532352171375, 29.92842772344721, 32.97385192049303, 3.907892548715129, 54.68830756856171, 11.511820072802195, 82.80352121981606, 5.986516363240899, 25.94216400142446, 32.668034573739135, 62.17753632353639, 49.82082450892373, 86.0313002111631, 32.83438604927255, -2.1209016955427984, 55.47621844731185, 13.862408212011175, 11.426876673065275, 33.42455180536804, 18.02086343277372, 19.74669274657031, -0.6500609000871469, 42.59015040246743, 58.93313506170324, 19.48224032577278, 133.82843808006479, 16.377304937605174, -41.68281766460139, 73.77058870105807, 69.08795262654041, 60.134891695338965, 64.11263202293088, 23.752970779564894, 50.51150503570393, 61.80389105117726, 55.347927750257355, 76.27263314008722, 53.12283711724271, -49.30431454593349, 69.97138826329574, 38.140895314017186, 35.556277539122256, 16.347263019368473, 8.240055164821072, 17.447808332876434, 7.803335152488579, 26.39244770649188, 29.99123446666153, 57.40370678858557, 59.200743120410635, 65.79986058892486, 40.55399490604617, -4.648277159166696, 56.516582685775695, 102.22805817143009, 65.70911984261365, 66.12377631167746, -12.8575707983874, 34.67470936022487, 37.19930613909483, 74.05452373582708, 34.44293929441924, 61.59543947203415, 46.611275420360386, 33.56380225362827, 53.497288661735, 83.71480966165673, 42.51382181026899, 46.0959449355782, 109.64740809318229, 6.844042386797277, 19.38790195029796, 37.68489557574859, 51.01121289259734, 49.243191615070536, 14.04300935074348, 13.554029701593734, -4.355078082413876, 6.994909010013979, 0.006465603381735852, -0.7073678360377311, -0.22142063177019092, 6.32313177463897, -0.7680036272731873, 2.544821827831629, 12.092953586536867, 1.9220926583065605, 13.520012542175058, 7.3554675853251466, -1.8718756791343196, -4.166491129809884, 17.31369429215625, 3.9468777550762804, 7.566907158541841, 6.257582499971912, -9.504472370468733, 4.012466545177918, 11.99165298870517, 3.1974195366463256, 19.27572088293089, -0.6504724308270617, 0.8235081619684905, 21.747287549338736, 29.41121487160468, 41.12017678489222, 44.00366781410379, 33.79644880841145, -1.0416746752785873, 54.416226643786985, 19.68223414130889, 107.75933038853776, 37.73892765227485, 91.43709466025909, 24.053603406363465, 0.6176131589115172, 78.77358897737611, 8.668717773363138, 64.06075168057325, 16.05386927539584, 24.220642510553944, 5.064905893910307, 19.152297582991647, 8.783799489209866, -3.9362246267811942, 9.229971915962418, 7.521829421507637, 23.139029631078643, 26.122200042144215, 12.772582287610582, 38.648703521637955, 2.496853180135929, -26.864887134970033, 36.63565938689057, 15.583038010856173, 24.290796723516873, 1.2940265986527117, 26.09556206026719, 31.712644969422115, 10.044719606387417, 54.03900585120124, -6.3110885926225535, -11.518404080345295, 35.09171133534829, 17.624756625968498, 30.870021434965047, 9.593131258011763, 4.246599906867418, 11.716546464558407, -2.211047451674343, -3.5581854670152695, 31.162558556801873, 3.445737324236788, 34.757418111959396, -4.771069502716915, 32.488376537975114, 9.964780122615508, 66.60626109020635, 34.12811639726285, 26.000611542661602, 17.28221094829033, 53.277926185622974, 16.889372804409284, 50.495680914656084, 27.95944924299561, 10.819659525025529, 3.4471486394216715, 38.16886705212053, 17.77750163629493, 41.43478208566055, 24.3349978711405, 25.807038241196373, 4.778221612020555, 32.97982370895788, 27.671287661044865, 36.33117666488438, 15.425105197265399, 22.609392425592112, 1.2657839231663606, 21.18222156317845, 11.346345625941538, 7.030133424805613, 23.4003404841613, 7.289075253540695, 30.083178735034952, 1.9943455056786767, -0.16105956022614976, 7.472924943303621, 19.05259941210217, 80.6464934900781, 17.425374375970236, 84.414467874741, -11.008211324765192, 16.406982664285977, 34.47476779108454, 57.093980953668236, 43.14760440449288, 21.441544164640003, 31.43273359035991, 32.92883338581791, 14.054354520920946, 35.59068725763346, 9.872122195572558, -19.81324247309916, 19.032676243326854, 28.121335497561397, 69.03586648894014, 9.57358200998172, 81.29677046333134, -1.0555684256197853, 36.07392850765805, 49.14316208610698, 80.10152987755167, 33.10939520382726, 2.892186772534309, 55.04451552814401, 42.186160295034014, 39.33945492037356, 27.46908410771057, 18.7155702951948, 8.061160369928007, 10.479309235187358, 14.620701830389095, 22.600245539205332, 26.205745248961527, 5.837965530808266, 3.43923442257637, 0.6268039750207977, -0.9191760942286671, 0.018392599539770293, 3.0522505547705454, 44.17926714817397, 18.508652651495694, 63.08128168681982, 39.65289003718992, 15.673138492987874, 42.16172756488115, 63.01760199780025, 16.436057362347924, 52.78230295456408, 51.40839272691102, 22.69470180585901, 22.046633998486328, 21.148662859443697, 30.67015960158072, 15.777047617356963, 54.77974911894735, 16.690988796836137, -35.78577652848848, 35.06667080254433, 30.88394953533097, 25.09083335574485, 5.717727408854852, 23.554011519799054, 0.9189022689215127, 7.370088681320034, 2.973730746545952, 7.802626425951509, 22.61518609609043, -2.3868396975845925, 7.2245209717050685, -4.437042874781349, 5.469507329011355, 15.695168148308621, 17.81208985153602, 57.77841879017971, 100.21684050918375, 19.384554015109345, 139.60407229087187, 64.38276653878097, -91.05621955505133, 132.6857093212493, 85.60371048102519, 51.81836602551998, 0.4619481179047398, 41.322587469239565, 31.665561154409083, 21.33724550104705, 22.6030004566843, 93.79456548232022, 24.454172791792928, 58.80529939136984, 17.90254523531232, 24.533786853449556, 28.777402705653582, 102.98865440926429, 79.2997127578851, 92.69492022664852, 19.953624874875395, 19.50590167384368, 0.018996909839209764, 54.42950283557491, 42.84926501437058, 36.339471236008805, 15.94083077339786, 6.392647435590318, -0.28302866462867016, -1.274685371104748, 4.113893280841659, 5.569804345438074, 0.920241966304411, 25.010266792521517, 3.529886009276403, 32.84271652611038, -5.94991226642371, 4.5022952796963835, 52.59871132343169, 85.72627840771023, 57.277996230200145, 182.7074782478083, 37.706060620560606, -6.770504092610793, 116.69779208595695, 31.641885392272542, 121.01969735686394, 80.1466362184066, 12.39450889200672, 44.59260013110173, 38.53291738180253, 18.965810955671905, -3.350026338423222, 19.753382273331695, 32.69986653209591, 9.778510667052842, 34.70828359840754, -6.465033167329313, 3.7138057435325464, 18.853478385446422, 58.057874402316884, 46.86557179926706, 55.942007788579396, 62.72033637597456, -16.583865549535545, 12.72619362329528, 111.21078608696048, 55.60501985401011, 82.1485784017176, 95.91745205998913, 40.973214711858475, -42.37252096937762, 108.97037920902213, 126.88559017314775, 81.86008239505449, 15.335992465378297, 99.04530229691717, 36.85553668415628, -41.308726010982376, 83.8782754569334, 25.934020480178187, 36.427630521371526, 10.35991896584109, 9.011608041690245, -4.352817792800192, 4.316404827751952, -5.340065384463507, 8.242413797386435, -2.4845309756991956, 12.523652126507688, -0.06252683515623403, 10.378654459896891, 1.3367323077594708, -1.1966893977601387, 1.546042360603, 3.1436415936865667, 9.335943144627583, 2.2027710056402015, 4.61209399244789, -1.868715935673455, 29.631969683600808, 58.379599964451714, 68.92670691563194, 49.08826685070028, 77.90290277099481, 18.714408263464577, 2.5942458448801275, 86.8867403643425, 71.4368557154342, 68.72772898641925, 45.478150452238, 68.93046612913157, 11.432615079234463, 13.343185991686, 36.98658585739115, 68.55356898911748, 32.64174420443054, 88.65552053375878, 15.483638457038296, -39.31803348380786, 42.81150940840959, 35.22599007539717, 41.97231539606012, 8.332305382533285, 35.43707703495869, 6.22512160515862, -23.55951299901214, 42.902152844781476, 29.781700165217732, 24.176669919920887, 30.770181353969825, -6.620125567905006, -7.443929564747687, 17.905914004347956, 27.843462108112732, 12.649259582662982, 24.49333552991951, -9.300759595121386, 11.761268693081284, -4.523995514072666, 18.85913150513543, 7.943767885830728, 6.51932056537826, -3.661243091047602, 5.893832186337012, -3.8715750780604266, 6.82549788303665, -6.012382719669137, -0.8632917073912325, 4.712183365175851, -2.930985384782601, -1.3133087224725999, 5.1237265033950035, -6.308609569986237, 16.220213364048128, -7.137838944608063, 15.982131558368682, -2.8699722204318623, 5.493311115548593, -2.678512296517767, 11.99375710192153, 3.498213497658865, 5.885467104237104, 0.7245570849949254, 1.4154605793448627, 0.2027455425120308, -2.006392800049944, 12.43636079162769, 9.341974820843074, 7.949314658131467, 21.487745027046127, 3.4597604644543907, -14.296921366230979, 17.583486156179344, 15.637537709226505, 13.193415454839098, 9.687350103553477, 9.213421061084457, 11.112015535327554, -8.728659684564931, 11.657009216288035, 8.529748100348861, 42.32017423872176, 76.47418589110247, 19.26113145601596, 140.61769492777182, 22.632842822322175, -96.72139662389927, 94.31423083902538, 59.540634043170314, 43.59681237943474, 5.334803766619062, 17.912000117357486, -1.1903972237350593, 24.4825778716894, 23.853765097179505, 52.79707189482944, 4.518229591100216, 90.41786829170795, 46.54400680242247, 2.2158061630628367, 81.25630617403516, 55.513485996123464, 24.353054875441444, 25.208098466430016, 47.04911795243953, 37.61622744256682, 10.149210516666031, 9.893147007939668, -2.658623291558018, 1.5486334191966409, 0.5158593804124243, 39.22038458286064, 43.23704608318188, 28.96561306091637, 83.17552615621766, 5.922355392228724, -60.59788116270748, 70.99240146915406, 48.10047068961764, 35.714499387590664, 19.310633009956632, 7.444158646429045, -10.15608238352738, 8.827483432007645, 4.647470282852941, 6.80930140936427, -0.2917834205557237, 3.013978406106437, -3.093221576497184, 6.16394111658462, 14.719644391527574, 16.11377274923909, 16.77723651131097, 13.673936306341336, -4.301735358810561, 2.861955331675805, 27.487940715695743, 13.402024068795408, 21.280760256246968, 3.140459047987548, 12.377359935618022, 23.06150931935136, 4.841755922972599, 34.198565324896315, 4.742148138204627, 1.0453715910444465, 42.94747500058194, 23.779329954954044, 102.32011482258761, 70.77156448840907, 15.318542979620702, 130.70828352116183, 44.398150857325675, -1.4084925108554103, 75.3618316946967, 80.30847323687054, 27.81646256035458, 56.546795408539964, 27.88772862931947, 22.553227877859776, 12.264812131834455, 0.0017856572017933559, -4.8179218903084555, 41.11027352893109, 40.973462842135994, 37.75736466412853, 33.90352690711637, 15.762516540497316, -7.837431076259236, 19.17173433237438, 45.09547692896651, 38.456203976540806, 17.051257705646165, 17.507633857467177, -1.6785050967823878, -3.7117026490028007, 9.69252056212923, 14.426373626092357, 17.81572903683071, 37.815966974244624, 51.920299086935856, 44.85247592809091, 64.63479577887603, 35.3023982050545, 25.35003596573617, 79.97658845823003, 111.15384288221294, 36.56972940181292, 133.1138987121711, 25.448049931761943, 64.24765943474753, 11.75713800088339, 102.34773182190422, 55.16648770107611, 104.4777731013371, -4.514782246148037, 26.39812737905345, 16.469486307070156, 43.50300569861339, 39.02018288493599, 15.480457838337529, 24.691860149165848, 7.375347602362581, 6.682759808726374, 13.083833087794922, 20.206869642799592, 5.065261589351742, -0.2586591359178172, 17.89091950668944, 20.341243226332082, 7.809082990174339, 24.212832671002463, 2.2959096396197918, 2.9766463596117063, 5.648388865791663, 19.842998237156312, 1.058176538367283, 9.811419370417877, 14.867091802469385, 2.9490239214814142, 11.786126797133097, 6.744917415106482, 2.9136694682618582, -7.892376211297086, 11.324180912346693, 5.531176517951631, 16.666995317805803, 28.803951268006635, 49.822252980947255, 43.180289732804624, 74.76015395004957, -39.77616402290394, 73.97588184977644, 98.17507257667489, 155.26641937886586, 112.99067225001554, 72.65314992789837, 114.62651830814195, 27.553587683649596, 105.18659570452664, 144.34504358575776, 34.52389157553515, 141.80151029493445, 36.59496944207598, 7.3006022911398105, 65.51325752072178, 75.6691567799474, 18.090750083710887, 21.55737376311356, 16.809220574586192, 33.36485438856487, 30.89100489150143, 51.16106245978642, 36.9557741590551, 39.3253567796601, 44.08778702057403, 7.674457554997588, -20.809727096104474, 54.55766374980373, 46.3024250123339, 32.468906450076425, 9.266022594131371, 10.131302992511767, -5.833691140303692, 9.675771187973977, -3.539045499833699, 31.7762888099611, 13.116946894792747, 15.19153386742368, 48.08035727283814, 23.78386498524742, 8.045193633780364, 83.76663517796749, 67.06368260716047, 30.219833090851907, 53.276602204898126, 106.63623794328177, 37.744918761377534, -44.70904891594654, 65.72269647958227, 43.20529175227151, 27.622588313520886, 61.52917711735504, 57.737971371121645, 23.01844951219799, 105.59476206073961, 11.008794053461315, -75.12264493703458, 85.11046980451576, 50.37657243927445, 37.46857627284515, 16.4082307282052, -5.501400674720812, 20.726446215684646, 23.104534218916523, 114.74293906873525, 87.33324008808557, 136.9017269844121, 110.57994167526388, 21.719863177076377, 9.661276357674733, 146.1806001684136, 73.68189825551906, 131.26301955421553, 66.055951645792, 52.30076813594752, 38.999266116522534, 24.858425844256573, 33.66126339631839, 69.06479968505148, 92.077381993627, 0.5592290202439614, 19.54957816107168, 38.07497819998525, 93.17687063953463, 41.75724524818638, 32.848189295697345, 38.63191827853848, 9.031150992740862, 21.549016524112652, 39.967281067085004, 45.60997075114037, 21.961291832559425, 4.723955018844524, 28.06603657921265, 33.07360148571891, 15.159891524437306, 19.611745876973146, 41.70397147481876, 44.29579169720068, 67.86348840942546, 29.32229352094491, 8.591438721628599, 54.75902903256797, 48.39391604120524, 31.655324762526234, 84.85583214923804, 53.07102772360339, 28.56252935757695, 118.02429690109022, 31.066252346266708, -66.05771627584411, 72.95083937970921, 40.58878787980917, 32.147238956880145, 9.245983539018159, 16.94921578360014, 16.531011325819847, 14.637674873153944, 16.78353714937663, 17.864482426840198, 15.676087058953636, 59.07878025676008, 24.20045144760485, 7.258488937434333, 38.694476088965004, 44.73516376477194, 10.756135293805574, 9.641575574598122, 10.142627492868113, 45.69776223757769, 38.32557932155065, 43.43857398070303, 21.85329109802751, 20.145125964465322, 15.448391081835958, 13.062903625143914, 49.271622274351, 25.555348776827508, 7.0888508520495925, 22.93426378033, 48.86982816788199, 62.822770347016984, 32.65371737590681, 87.41355476798776, 21.885657281798075, -20.4457259767673, 68.7976533392972, 18.00901642965662, 60.83966391411159, 32.20467089731572, 28.629932841606184, 48.485758175815725, 42.32479444264172, 34.66308555835805, 78.58887151202794, 44.82858758141808, -14.141671004591323, 64.55556551195548, 15.55301320635041, 51.81477019763659, 18.404291299600082, 11.440820887733587, 1.837945718284756, 1.844782311737874, 2.7881620670851026, 2.2929663364497936, 0.22668145648837945, 12.162789831723103, 15.20784610835905, 6.078000547189735, 38.523694861950624, 8.962444577849269, -35.26293753723564, 34.79980791644361, 10.63921288129215, 13.287832994492334, 1.3701859637051839, 2.004472660576919, -2.2994453041639584, 3.135285265302594, -3.190913957733535, 8.534646768741448, 0.7662883824617399, 4.988209035437839, 54.24149818237048, 39.33873193820996, 61.36241014859462, 54.360467740825854, 26.37703188362471, 8.95767197903939, 47.257474597599206, 55.809435980314056, 50.955786158279615, 49.246105830910416, 8.399008383420053, 20.743336074938757, 6.28926979417567, 67.03317689401679, 47.82709527020431, 78.24246447241896, 64.18108479379524, 13.173388352858865, 30.759070360684014, 84.81771426423376, 47.408031816644936, 71.33671438906347, 43.57237111236974, 47.418001003696396, 44.884008400970174, 95.55134789620796, 20.597787147436208, -44.273595066481576, 57.904617364679275, 36.99514706140724, 46.19662983593855, 2.305501338693558, 11.351451004854399, 22.275610144293925, 15.307885288386991, 22.786368534999045, 16.533565869969383, -3.953982234019435, 4.201753708003017, 48.174866948710765, 25.738164160902983, 54.595202852038646, 21.51808929470862, 33.8466562543789, 32.391342379485295, 53.89386033987142, 29.283428122641737, -14.020344589886166, 58.0537525293318, 16.731738973992357, 30.25200474357676, 18.84844637752402, 19.884356142440375, 17.76631755826184, 43.56823327640857, 0.8948562322055693, -22.573874647005383, 50.64405017121968, 43.58158488556097, 73.57643672652236, 70.35493354459592, 27.72628734942971, 46.13227858827831, 44.99576461204137, -30.551798835440497, 80.70864995436797, 58.229180036493474, 65.16679861506648, 37.72607674833414, 72.11896657117302, 12.595169913263504, -6.641526014917652, 40.17386556568542, 26.744741005332813, 47.53039822587293, 16.997459475151423, 16.085401262758875, 22.432399913475216, 30.260944655992486, 21.3089202187124, 47.53013522855612, -2.5584846999944517, 12.90781852078172, 21.228818478543385, 34.620692459370694, 42.162901948646336, 44.4764068272525, 33.18783463955296, 62.20089361667338, 4.624900767512258, 78.12037036868887, 21.424384260210722, 118.84106942011255, 53.71308220879553, 61.19453918150617, 17.980278946907937, 57.19473770027028, 32.43010466549426, 44.9779071409325, 35.61304876443677, 8.619601878521827, 12.332758416287124, 4.366922831457808, 6.505943002941622, 13.338533818657242, 3.7272661339831075, -7.2647260080504426, 8.461091893567191, 4.804943494813092, 7.455520272399159, 5.6926952581884125, -2.866181063649031, 3.2471577961908507, 23.235803660991273, 19.281352143673644, 48.717518683133875, 62.68926357707633, 15.815783936904282, 85.23594154093068, 81.03843832572967, 3.4130888201204215, 154.93355513914685, 52.992902544073075, -54.91999608737493, 82.24181082967712, 46.44145678864817, 77.43935465504657, 37.128596011156084, 46.106086682127234, 61.52151518958953, -6.335775321962814, 38.1413702265057, 85.86721240915924, 118.14750775573302, 43.06691911515151, 14.826458193083852, -5.650270444325262, 73.90312067668577, 58.26326854967056, 45.428152278089705, 10.154707749857337, 55.79052990038561, 32.13826013701258, 43.757492557838354, 73.46770257664679, 22.477821049995896, 43.56618466362, 83.08050983543146, 60.89912349745458, 27.290178669787878, 47.9838857522813, 25.295609225429384, 35.25946281257682, 23.444628342992612, 2.869921141197726, 9.24024720516195, 10.962494124879878, 13.422789114940109, 12.483530656176189, 27.101878824404885, 40.12723746709253, 2.4325937888915448, 66.85653189710656, 126.2217707288373, 47.86670655972523, 53.526867512404294, 61.877565820747634, 46.29867532634506, 47.278820748244044, 83.79993929386757, 58.94518527364579, 22.145177829113504, 29.455723898905703, 14.34372047024564, 15.150468615889908, 8.472097401243085, 23.561614568379866, 8.698373489751468, -0.97634334295598, 29.31803210435376, -0.1264053077732683, 11.036605491903668, 9.890468281612879, 41.318264795480076, 40.82178113548597, 22.962980985655115, 87.5707329188046, 24.223269184722426, -40.94206561447963, 79.04222011292873, 30.173955428929233, 19.901520280448207, 28.910360316328262, 25.04269459388642, 34.647844858882195, 24.685713352985232, 24.621729533515577, 27.63381480506614, 4.477394031406419, 15.88600443828015, 50.32037487068083, 19.798740674684154, 5.9300564770692725, 16.72530413798786, 13.110483464937456, 7.984791449622441, 9.226293209922712, -2.6274591821485993, 3.904942175683779, 6.462668298492456, 68.52934860054215, 9.8379772436044, 101.26935256761742, -49.45672165635477, 34.317502209711336, 38.36630142966161, 84.72829324727127, 74.29422699654992, 75.73016360757725, 34.324875640396854, 21.002356185251756, 83.55660873693235, 27.41999241560984, 0.40698740066675754, 86.81284045787545, 27.652789471434758, 58.177481812421036, 16.182174147249214, 41.45545722611422, 7.832536096186036, 45.21510485723687, 9.72772750964579, 41.52000500831823, 10.74138854440961, 36.90036938756873, 16.25448650509089, 6.618362695395106, 27.931927905239586, 37.12015322437155, 31.09650242900925, 35.695668564319234, 2.8838534792846815, -10.095006897269403, 31.87367155032203, 25.07706125614531, 5.279101523776874, 7.477663327775023, 12.59081050900345, 10.883301525946706, 22.17941320757675, 11.37112983130284, 22.790281268167558, 3.052592431916665, -9.348362038741193, 22.569570403747, 14.018996418218766, 9.825622883935033, 8.079176839864086, -5.040060215099771, 8.040557792794262, -0.8294964827757352, -2.212729595636943, 4.205743915207208, -2.9518210196693193, 2.3215388236254624, 7.545573686533719, 6.9304869971546434, -5.386972328036665, 9.939745956891468, 50.93001086795334, 6.307798082646855, 79.0782178117988, -25.309253268304392, 38.03518322441528, 31.244263346063235, 83.22259224967652, 75.40797441269771, 29.160796056477714, 69.2357788739402, 96.01345665539996, 64.99364654555346, 86.87738232000942, 72.79589441530254, -3.232001209644764, 144.12760341145338, 65.36200557446791, 50.749296677388, 56.04305127075749, 64.73119087720977, 65.97877900432994, 123.17561912794216, 26.913308340540425, -50.934038851515396, 67.68239447796469, 54.990720368734415, 41.38778657394439, 9.952876139735189, -4.0916726293390875, 19.461362768920083, 14.291617626145847, 2.649137103837832, 24.075899229610457, 11.935485772808939, 35.8906520146915, -8.966084628266843, 21.937910646590865, 4.73367905896454, 15.978826475460256, 22.066111896902935, 7.309246017094667, 10.504774068849033, 1.5214257704534044, -0.7354005486254058, 3.64059655844802, -6.179903609643432, 7.0851190749251876, -9.018332517544234, 8.224017869466204, -2.187685250625532, -1.6888293456868524, 4.0768859140994405, -6.077732072153763, 7.784838799953696, -6.614102024850676, 14.346121755987788, -5.31213690709759, 16.3477852586338, 36.61834993728742, 14.174834485767349, 43.2522672646115, 33.005038843478424, 8.772245340812589, -19.663093581891466, 66.07252636644566, 32.7009865749515, 52.077344837041196, 9.546189647940082, 18.276237316031008, 14.461243053270318, 12.285527663962256, 11.351020600546637, 27.863172887190334, 62.38710243453836, 91.87862358711055, 73.59668192913944, 107.69912754205458, 59.21335940972142, -15.08711401399114, 62.93130604541872, 178.70802295872954, 121.82321617127218, 89.16297853334058, 80.44923300913051, 30.26076780827529, 30.673702463970898, 57.65102434943625, 67.01904844547163, 45.16414333799011, 18.33271310276165, 3.4760241143596593, 5.268320108186749, 3.802682995484542, 0.32874532618231456, 11.948618451751305, 7.784078796512519, 6.207104363602788, 8.693326145210358, 0.5228291559249953, 2.331390068435942, 15.706437819979396, 12.505212292906615, 12.113418638002166, 0.9600785234448916, 6.177877813868484, -9.820550611842478, 14.102261363570813, 4.98427176692281, 0.6278173181661135, 14.96032922089128, 24.579637335332443, 28.6276816271926, 18.64033933017981, 46.41534584160489, 40.40059995695157, 43.33067958394393, 65.1507934617832, 115.27061749752066, 20.0018664701945, -55.3451270672155, 91.41456541786388, 42.941153871428064, 48.44106099700177, 28.292144624345543, -5.67461738330746, 35.96516239138824, -8.882063305671757, 12.134090841437754, 3.2822222374646985, 35.154733555391225, 47.67373281919237, 40.42310698854999, 67.69867909604142, 8.424247748464637, 50.970688817195835, 81.75341789143422, 153.2306434440982, 78.43893364024532, 212.80864837481627, 25.859105075167463, -20.41147753677376, 88.6534477732744, 112.50818700622877, 83.63549036925734, 31.92228984884474, 22.39857839635266, -3.985411185800136, 8.674821125198442, -5.406286907957423, 7.781487637270766, 18.330513285978796, 6.093481351280303, 25.436530284141217, -3.1788275202091008, 1.9370186001020073, 5.397568968612608, 21.247526625474023, 13.137123189595346, 34.64961801202762, 4.20918661099018, 37.82053487493101, -13.12408435782973, 14.930420809076836, 85.9015412180108, 88.2195703523591, 96.10149313908803, 121.53379310204397, 17.928123434361623, -14.318095850068474, 168.10621574494334, 104.97955987595249, 122.55168097227721, 118.87931678628328, 66.94917391821281, 19.70000031627559, 69.74746934797622, 15.983994965911268, 74.79806705358662, 42.04428503818899, 25.569589026811055, 17.69489017539101, -4.2761590732217165, -0.7866938329273775, -0.7788963811717828, -1.643382284006758, 3.247418916937293, -0.9728492524410302, -1.4448513343186653, 14.065273305229432, -0.4253287199329101, 31.04300671985435, 29.118011436402483, 57.352010094937214, 25.97137627057232, 59.04794767280001, 42.228507435511965, 66.167151046481, 96.40328368399781, 124.2847334666717, 172.44178743407198, 85.33487053132767, 118.41120135480463, 65.47884911888991, 43.94882484631168, 132.38521567497327, 74.73456165985324, 78.46539351511204, 47.93385940734176, 38.56299221134002, 15.29031996547181, 19.356724358311165, 3.9772030711649755, 7.722049785277548, 8.215068981482126, 38.13361120720984, 21.388717636451393, 17.106454765020427, 25.191268536432446, -4.108620612947959, -10.254417996048382, 16.153715067358462, 18.182198721522656, 3.103279109162809, 4.712953969387185, -1.5957036734340577, 2.098958934173045, -1.9994958138929457, 6.563543284129998, -0.9858216521619152, 7.568588545701774, -9.179407421117357, 14.996850552177865, -3.421289611894194, 8.433295314910191, 8.924460836063698, -3.8862528829293694, 15.763904304881244, 17.413697208574522, 1.5430478413407478, 40.39959031923807, -7.492801708165544, 7.035552536036299, 13.674946575610287, 21.80321191079493, 14.206428750021562, 28.83889013629031, -4.232964652220261, 9.020003324314025, 15.93532490800925, 27.001431294044313, 14.279617841786727, 28.628399490114532, 6.009698345983196, -24.063895463982313, 33.95405997840902, 21.36067996494925, 16.22277376645542, 23.019308087791792, 5.830832042401973, -18.041027195622426, 20.753153580180992, 15.87828905334037, 35.44046087126047, 31.24736239522142, 13.133657865111068, 48.50361162427601, 1.79108217440006, -26.093654866459413, 41.93737658614083, 21.405648433307764, 20.239694935912638, 18.767412601932612, 8.148915628848812, 14.328008478369636, 15.886538029464521, 7.294175641014618, 2.645356912375137, 70.97118457846332, 41.92322420754764, 57.631345792740035, 43.528981591069225, 8.683482832491563, -10.727127398982375, 66.51917783962378, 31.311020375892234, 45.636155465326986, -2.700638898723695, 9.3191064054738, 48.7398325506343, 50.15047610440149, 35.09800363001622, 99.53938827880216, 1.7392757456290155, -66.13647942128236, 84.40953676024715, 46.8045476878973, 38.877128585330645, 5.37598241531449, 5.421961595518451, 29.04739476201195, 88.05026246833552, 84.50541966314611, 83.47254429817332, 113.8923844690552, -20.38592584582119, -8.92018298525829, 126.1854712565301, 75.26158421316053, 52.904734818872825, 21.77707850140111, 2.524520916337792, 11.641980984801052, 13.869845874806781, 6.187964235346833, 44.003179836852205, -8.090770867063405, 33.36640161625962, 19.657584199603164, 44.5865559012356, 44.20503676979208, 37.19845864398009, 30.03247294806843, 17.121365051833713, 51.7969027449633, 46.08623518467181, 24.422830995107944, -3.0985246062372873, 55.40905386319307, 47.94480005760104, 25.00343578881413, 41.81252271785111, 14.09237550054047, -18.42468765293481, 41.87617649585849, 24.11260587859449, 20.806811535623144, 11.899473029987194, 24.21943874072003, 29.995564476861105, 26.05913994463289, 27.408039867068098, -3.4194773189944243, 29.358874059992146, 36.80401024396433, 41.65442656544945, 51.51484838187478, 13.33815187993116, -16.422597690326825, 33.95955689541153, 14.1248752877812, 3.5722052584796473, 10.484272772989984, 10.268227325649995, 19.666736978954898, 16.255017030740895, 25.92036445944803, 12.673608614197791, 8.305501202882738, -18.56690513403647, 35.76784598126739, 53.44664834817479, 73.20663576448212, 37.72987000043884, 85.84230220809391, 22.29569228053066, -47.95670817522033, 54.59078309611813, 59.74466579918959, 42.46442772837392, 21.302639219560746, -1.5177879616120165, 18.13935318755995, 6.383721418168125, 12.034576964997502, 55.69887544460865, 63.30583518953023, 32.74449321509351, 137.8151758702304, 23.67955985951272, -69.23419549444708, 97.4936062601588, 72.64647832716389, 70.14296042364504, 40.706079383278116, 17.305993726602196, 51.9441097254303, 10.347678510112132, -13.584211201821418, 29.85166274289208, 29.776086697352905, 79.1288567007393, 16.574810552841186, 86.33490140240949, -29.995713229182456, 15.863907425675961, 18.154591682239467, 68.26838215303164, 47.15725953605393, 31.661258727107207, 16.576025073775774, 2.7050469004545405, 69.85599738584156, 42.4612462696567, 119.47926103619032, -1.7226149599489489, 56.3919436891762, 19.104076236773366, 53.51063090147246, 93.02369057142354, 45.47675020237481, 72.36884941183587, 54.39041990278166, 59.64182239835858, 89.28041572300779, 23.297234145428092, -17.097410806007606, 103.13493311177481, 45.231904330274446, 21.649396841606936, 32.60243651780794, 29.02602450237904, 24.646248745869453, 12.440289731595787, 24.917384662865015, 6.479979333001552, 36.162634809458766, 51.47604352631389, 74.34563409032113, 53.734835769172264, 32.760694268912815, 67.61402858823851, 38.659449010348496, 126.65970024316317, 43.61069496631673, 20.431324705258646, 13.745385059543398, 74.15873421707883, 45.427321106457285, 32.05200388193486, 17.199610782826607, 3.1264868671289285, 1.0661214018630534, 38.05458249467106, 21.996755045993282, 37.094403537409875, 14.785431345865142, 1.4868391310972129, -8.816618516645761, 41.29109525099834, 24.509840003767263, 29.765563528435692, 14.719893651353207, 27.268078770106115, -7.732227242477592, 38.856993259849474, 5.9271378575013856, 3.1897302874607654, 63.388026191208226, 16.65104581974669, 32.271540371770065, 63.5501842846603, 69.067819343113, 45.775002812530744, 103.50178134173176, 26.263985989914687, 17.025508447729365, 73.4239067865752, 99.96864671380274, 35.503989961582505, -1.6721036801789841, 46.49195678790767, 18.69568394805295, 17.884237539179907, -1.3974429942760231, 5.957274035357295, 1.8932572881282455, 9.856899033297934, 22.98594611065204, 48.38887779594102, 20.206681090699092, 80.89570043164488, 32.68412063208592, -54.98472495060804, 48.64801322535282, 36.80702167162214, 41.034850285583786, 11.180444541643816, 5.545380356642463, 9.490381517400499, -2.4494810327495404, 21.051365407226857, 7.016891987927757, 19.122211947595872, 4.443746410990073, 0.8178881032340541, 14.235480315329047, 20.902481912909476, 5.913668126370162, 15.237291407451364, 4.31399777470444, 4.029029023928898, 14.364912301003564, 8.435535018315882, 3.0501777900082914, 17.936140841916206, 12.780675024846722, -9.190111795787262, 24.532870239441962, 17.79798677544583, 24.00580017679865, 40.15682162707221, 50.49375104559885, 42.244745603918616, -21.565362076248768, 57.668501108597745, 22.922082486789392, 34.678344079560965, 34.82925245627705, 35.51126866396879, 26.689318409976117, 15.753292670910724, 34.91506601529508, 42.95809559454358, 17.364484849048182, 16.449709027752533, 63.08555910681524, 26.0423725891455, 44.52431453205919, 20.716181194008186</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="D5" t="n">
         <v>30.03758037555496</v>
       </c>
-      <c r="F3" t="n">
+      <c r="E5" t="n">
         <v>34.04036099469235</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>[-0.14952753315459036, 0.14524883604941738, -1.0289050057324118, 2.2105101993677145, -1.4833859808145358, 0.7025099711730591, -0.3964504868886532]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[[ 8.93082432e+02  6.36494911e+02  2.52252449e+02  6.63873200e+01
+   1.04063409e+01 -2.12476845e+00 -8.25011634e-01]
+ [ 6.36494911e+02  8.80648023e+02  6.34088262e+02  2.53267862e+02
+   6.60193857e+01  8.25506187e+00 -2.69434481e+00]
+ [ 2.52252449e+02  6.34088262e+02  8.96678486e+02  6.41100195e+02
+   2.52652118e+02  6.37363901e+01  9.45689599e+00]
+ [ 6.63873200e+01  2.53267862e+02  6.41100195e+02  8.92618237e+02
+   6.38987648e+02  2.50655347e+02  6.44440354e+01]
+ [ 1.04063409e+01  6.60193857e+01  2.52652118e+02  6.38987648e+02
+   8.92646024e+02  6.33435711e+02  2.50491950e+02]
+ [-2.12476845e+00  8.25506187e+00  6.37363901e+01  2.50655347e+02
+   6.33435711e+02  8.83313374e+02  6.33541253e+02]
+ [-8.25011634e-01 -2.69434481e+00  9.45689599e+00  6.44440354e+01
+   2.50491950e+02  6.33541253e+02  8.86006026e+02]]</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>40.03604706152543</v>
+      </c>
+      <c r="E6" t="n">
+        <v>38.27546277079185</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>50</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>[-0.1562909108046308, 0.15428518860541718, -1.0358630872615902, 2.217763291130791, -1.4908608555757894, 0.7001014115545262, -0.3891350376487244]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[[1048.196394    749.88831109  300.79722095   84.86655354   18.9606472
+     1.95072729    3.64117086]
+ [ 749.88831109 1051.9624322   754.25831681  305.17716399   84.43076986
+    14.58634162    4.21691832]
+ [ 300.79722095  754.25831681 1051.08305699  754.41871051  300.90570937
+    77.056274     12.05011216]
+ [  84.86655354  305.17716399  754.41871051 1051.50174454  754.92539775
+   298.62574415   73.57008669]
+ [  18.9606472    84.43076986  300.90570937  754.92539775 1053.237859
+   751.5202203   293.40866212]
+ [   1.95072729   14.58634162   77.056274    298.62574415  751.5202203
+  1047.88283628  749.04017586]
+ [   3.64117086    4.21691832   12.05011216   73.57008669  293.40866212
+   749.04017586 1048.45628792]]</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>50.0257592924174</v>
+      </c>
+      <c r="E7" t="n">
+        <v>41.73221539559243</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>60</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[-0.15618573599266114, 0.1492985315254396, -1.0201245743586893, 2.199506662660773, -1.4687800088778589, 0.6945423285209582, -0.3982572034779615]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[[1184.26267829  843.506856    333.93307671   89.45748569   16.89030475
+     4.11783885    2.87786948]
+ [ 843.506856   1167.30116479  832.45075328  329.12229908   87.49374241
+    17.45230647    2.33505595]
+ [ 333.93307671  832.45075328 1162.37166973  828.89594486  328.40671558
+    89.884902     16.85568672]
+ [  89.45748569  329.12229908  828.89594486 1159.25472713  832.3229607
+   335.41697212   91.70685641]
+ [  16.89030475   87.49374241  328.40671558  832.3229607  1170.97597617
+   842.12899164  336.09170102]
+ [   4.11783885   17.45230647   89.884902    335.41697212  842.12899164
+  1174.32340923  839.30652075]
+ [   2.87786948    2.33505595   16.85568672   91.70685641  336.09170102
+   839.30652075 1171.77523899]]</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>60.03490151692988</v>
+      </c>
+      <c r="E8" t="n">
+        <v>44.56947361368592</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>70</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[-0.15809240543350678, 0.14567815525649064, -1.0190222941569569, 2.1986350921874913, -1.4682045719693286, 0.6937116248406134, -0.392705600724803]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[[1285.03303403  923.9361939   375.38241416  109.25758422   24.57777442
+     6.63020292    6.33275142]
+ [ 923.9361939  1285.27249011  922.04091769  374.5160219   105.3683808
+    22.28476987    6.39215277]
+ [ 375.38241416  922.04091769 1279.47654473  919.45162891  370.64351862
+   102.98139894   21.23839477]
+ [ 109.25758422  374.5160219   919.45162891 1282.18178535  914.73592833
+   362.20265153   96.64457905]
+ [  24.57777442  105.3683808   370.64351862  914.73592833 1268.61411627
+   905.09126204  360.83405998]
+ [   6.63020292   22.28476987  102.98139894  362.20265153  905.09126204
+  1265.00025492  905.48469548]
+ [   6.33275142    6.39215277   21.23839477   96.64457905  360.83405998
+   905.48469548 1266.22455008]]</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>70.00550113122169</v>
+      </c>
+      <c r="E9" t="n">
+        <v>46.85559589062421</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>80</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>[-0.16021354550189745, 0.15079333435534142, -1.0188586502141912, 2.197802232069211, -1.4661630663559964, 0.6909606637071483, -0.39432096805961586]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[[ 1.35152797e+03  9.68158579e+02  3.87131135e+02  1.10357698e+02
+   2.53635434e+01 -1.95853398e+00 -6.29538202e+00]
+ [ 9.68158579e+02  1.35329129e+03  9.66948179e+02  3.90075523e+02
+   1.12040996e+02  2.25674829e+01  1.31919831e+00]
+ [ 3.87131135e+02  9.66948179e+02  1.35293569e+03  9.74084590e+02
+   3.91914745e+02  1.11094266e+02  2.58041287e+01]
+ [ 1.10357698e+02  3.90075523e+02  9.74084590e+02  1.36300450e+03
+   9.72767958e+02  3.87471643e+02  1.06484250e+02]
+ [ 2.53635434e+01  1.12040996e+02  3.91914745e+02  9.72767958e+02
+   1.34933411e+03  9.60508188e+02  3.83540750e+02]
+ [-1.95853398e+00  2.25674829e+01  1.11094266e+02  3.87471643e+02
+   9.60508188e+02  1.34374085e+03  9.67795582e+02]
+ [-6.29538202e+00  1.31919831e+00  2.58041287e+01  1.06484250e+02
+   3.83540750e+02  9.67795582e+02  1.35671661e+03]]</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>80.00328769999282</v>
+      </c>
+      <c r="E10" t="n">
+        <v>48.66085315520022</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>90</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>[-0.16426076541053306, 0.1498625228543782, -1.0126931093502356, 2.1905707007253246, -1.4574340812328686, 0.6877330658125881, -0.3937783333986534]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[[1388.87972822  993.15858709  391.35253583  106.62740336   21.46542105
+     8.19264178   10.43283213]
+ [ 993.15858709 1398.4908516   994.51743554  394.54579604  109.90962712
+    28.8681358    10.42915243]
+ [ 391.35253583  994.51743554 1383.70076086  988.27430828  394.49851005
+   109.35345994   22.14073784]
+ [ 106.62740336  394.54579604  988.27430828 1384.33844294  985.48080484
+   387.60759409  101.49363777]
+ [  21.46542105  109.90962712  394.49851005  985.48080484 1374.81480376
+   981.57373165  387.813493  ]
+ [   8.19264178   28.8681358   109.35345994  387.60759409  981.57373165
+  1376.26526497  977.5417714 ]
+ [  10.43283213   10.42915243   22.14073784  101.49363777  387.813493
+   977.5417714  1367.2961736 ]]</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>89.97546387337403</v>
+      </c>
+      <c r="E11" t="n">
+        <v>50.11089492235458</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>100</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>[-0.1546366364243046, 0.1368208435863422, -1.0048635288335752, 2.1826657148992132, -1.4490644720845063, 0.6884704831006482, -0.3993924042438173]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[[1.42356732e+03 1.01476552e+03 4.00153937e+02 1.08005506e+02
+  1.92800593e+01 1.30707030e-01 4.45408280e+00]
+ [1.01476552e+03 1.41115758e+03 1.00029932e+03 3.93188952e+02
+  9.98419684e+01 1.51027773e+01 1.39367078e+00]
+ [4.00153937e+02 1.00029932e+03 1.40216904e+03 9.97914229e+02
+  3.87136156e+02 9.84108988e+01 1.70033225e+01]
+ [1.08005506e+02 3.93188952e+02 9.97914229e+02 1.39690209e+03
+  9.93545651e+02 3.91116632e+02 1.06214275e+02]
+ [1.92800593e+01 9.98419684e+01 3.87136156e+02 9.93545651e+02
+  1.40458818e+03 1.00813233e+03 4.00299782e+02]
+ [1.30707030e-01 1.51027773e+01 9.84108988e+01 3.91116632e+02
+  1.00813233e+03 1.41420244e+03 1.00656048e+03]
+ [4.45408280e+00 1.39367078e+00 1.70033225e+01 1.06214275e+02
+  4.00299782e+02 1.00656048e+03 1.41223743e+03]]</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>99.9237204068171</v>
+      </c>
+      <c r="E12" t="n">
+        <v>51.13829918391575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adiciona os dados para os janelamentos e ocupacoes
</commit_message>
<xml_diff>
--- a/FiltroOtimoContinuo/ErroEstimacao/ErroEstimacao_J7.xlsx
+++ b/FiltroOtimoContinuo/ErroEstimacao/ErroEstimacao_J7.xlsx
@@ -466,32 +466,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[-0.37769776158504653, -0.35767167319809684, 0.17968945449856066, 0.8145602575006352, 0.27480292169683246, -0.20454695215897858, -0.32913624675390635]</t>
+          <t>[-0.3795932009879999, -0.35529760845099656, 0.18074043205399196, 0.8130444085261327, 0.2768674000703634, -0.20525192955781896, -0.33050950165367227]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[[ 2.25468611e+00 -2.71947224e-03  2.69593344e-03  1.63439526e-03
-  -2.37154436e-03  3.24993947e-03 -7.93160873e-04]
- [-2.71947224e-03  2.23669450e+00 -1.02909676e-02 -1.07938160e-03
-   2.95970473e-03 -1.56154308e-03 -6.44842157e-03]
- [ 2.69593344e-03 -1.02909676e-02  2.25336895e+00 -3.97587385e-03
-   1.32280850e-02 -4.32147783e-03  5.13154529e-03]
- [ 1.63439526e-03 -1.07938160e-03 -3.97587385e-03  2.24373352e+00
-   1.66203509e-03  6.86263965e-03 -3.07165972e-03]
- [-2.37154436e-03  2.95970473e-03  1.32280850e-02  1.66203509e-03
-   2.25318809e+00 -8.92843227e-03  8.55517103e-03]
- [ 3.24993947e-03 -1.56154308e-03 -4.32147783e-03  6.86263965e-03
-  -8.92843227e-03  2.24276400e+00  1.54092827e-02]
- [-7.93160873e-04 -6.44842157e-03  5.13154529e-03 -3.07165972e-03
-   8.55517103e-03  1.54092827e-02  2.24965761e+00]]</t>
+          <t>[[ 2.25116127e+00  4.90025657e-04 -4.09287210e-04  1.97575318e-03
+   1.55667231e-03  3.88682167e-03 -2.33280303e-03]
+ [ 4.90025657e-04  2.25116126e+00  4.90140319e-04 -4.09269840e-04
+   1.97571520e-03  1.55673788e-03  3.88710616e-03]
+ [-4.09287210e-04  4.90140319e-04  2.25116154e+00  4.90597484e-04
+  -4.10917255e-04  1.97545039e-03  1.55490321e-03]
+ [ 1.97575318e-03 -4.09269840e-04  4.90597484e-04  2.25116183e+00
+   4.89627577e-04 -4.10879867e-04  1.97525147e-03]
+ [ 1.55667231e-03  1.97571520e-03 -4.10917255e-04  4.89627577e-04
+   2.25116507e+00  4.89424760e-04 -4.10568206e-04]
+ [ 3.88682167e-03  1.55673788e-03  1.97545039e-03 -4.10879867e-04
+   4.89424760e-04  2.25116484e+00  4.88294451e-04]
+ [-2.33280303e-03  3.88710616e-03  1.55490321e-03  1.97525147e-03
+  -4.10568206e-04  4.88294451e-04  2.25115981e+00]]</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-1.386345677960707e-06</v>
+        <v>-1.388939536405891e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>1.63777058640036</v>
+        <v>1.637757343389531</v>
       </c>
     </row>
     <row r="3">
@@ -500,32 +500,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[-0.1292648401907958, 0.062036594434520205, -0.9211541043258772, 2.0887490566931946, -1.3205968171419362, 0.5751739744144813, -0.35494386388358695]</t>
+          <t>[-0.17807844092715552, 0.2444557908326003, -1.1503069468222034, 2.3473009078203857, -1.6675219567821613, 0.8520645795144073, -0.44791393363587323]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[[ 2.67781720e+02  1.90140135e+02  7.51462098e+01  1.95001742e+01
-   3.01585920e+00 -2.25344780e-02  6.95908453e-02]
- [ 1.90140135e+02  2.65356572e+02  1.89620384e+02  7.56250739e+01
-   2.01850123e+01  4.00657938e+00  3.85390466e-01]
- [ 7.51462098e+01  1.89620384e+02  2.69577240e+02  1.93649187e+02
-   7.80598255e+01  2.20444875e+01  4.36236362e+00]
- [ 1.95001742e+01  7.56250739e+01  1.93649187e+02  2.72067652e+02
-   1.92975423e+02  7.69592867e+01  2.06855813e+01]
- [ 3.01585920e+00  2.01850123e+01  7.80598255e+01  1.92975423e+02
-   2.68862776e+02  1.91584830e+02  7.65595873e+01]
- [-2.25344780e-02  4.00657938e+00  2.20444875e+01  7.69592867e+01
-   1.91584830e+02  2.67322256e+02  1.89088973e+02]
- [ 6.95908453e-02  3.85390466e-01  4.36236362e+00  2.06855813e+01
-   7.65595873e+01  1.89088973e+02  2.64532759e+02]]</t>
+          <t>[[ 2.93520836e+03  2.11613942e+03  8.49522908e+02  2.32327015e+02
+   4.69917679e+01  2.75624916e+00 -2.28533708e+00]
+ [ 2.11613942e+03  2.93520816e+03  2.11613922e+03  8.49522521e+02
+   2.32326396e+02  4.69913464e+01  2.75602889e+00]
+ [ 8.49522908e+02  2.11613922e+03  2.93520796e+03  2.11613877e+03
+   8.49521760e+02  2.32325898e+02  4.69911170e+01]
+ [ 2.32327015e+02  8.49522521e+02  2.11613877e+03  2.93520844e+03
+   2.11614061e+03  8.49522553e+02  2.32325624e+02]
+ [ 4.69917679e+01  2.32326396e+02  8.49521760e+02  2.11614061e+03
+   2.93521401e+03  2.11614328e+03  8.49522250e+02]
+ [ 2.75624916e+00  4.69913464e+01  2.32325898e+02  8.49522553e+02
+   2.11614328e+03  2.93521522e+03  2.11614301e+03]
+ [-2.28533708e+00  2.75602889e+00  4.69911170e+01  2.32325624e+02
+   8.49522250e+02  2.11614301e+03  2.93521500e+03]]</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>9.972063529513905</v>
+        <v>9.972065629298644</v>
       </c>
       <c r="E3" t="n">
-        <v>21.32772072037319</v>
+        <v>20.52870687351134</v>
       </c>
     </row>
     <row r="4">
@@ -534,32 +534,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[-0.14339454108469085, 0.11960066703238818, -0.9949803054570084, 2.1723204512071397, -1.4340851491821278, 0.670651331924537, -0.3901124544402377]</t>
+          <t>[-0.18162908373744088, 0.25341734916319975, -1.1594639014071773, 2.357526887974693, -1.681773371240436, 0.8657263258623715, -0.45380420661520965]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[[ 5.05233430e+02  3.59521213e+02  1.41835422e+02  3.72691888e+01
-   7.31522850e+00  9.03398774e-01 -4.08527618e-02]
- [ 3.59521213e+02  4.98091789e+02  3.55207374e+02  1.41522106e+02
-   3.84938636e+01  7.45866855e+00 -1.37401295e-01]
- [ 1.41835422e+02  3.55207374e+02  5.02425347e+02  3.62997103e+02
-   1.44129886e+02  3.69871686e+01  5.32898808e+00]
- [ 3.72691888e+01  1.41522106e+02  3.62997103e+02  5.13320673e+02
-   3.65379898e+02  1.43639191e+02  3.77415259e+01]
- [ 7.31522850e+00  3.84938636e+01  1.44129886e+02  3.65379898e+02
-   5.09426324e+02  3.64256507e+02  1.45017509e+02]
- [ 9.03398774e-01  7.45866855e+00  3.69871686e+01  1.43639191e+02
-   3.64256507e+02  5.10482666e+02  3.62599296e+02]
- [-4.08527618e-02 -1.37401295e-01  5.32898808e+00  3.77415259e+01
-   1.45017509e+02  3.62599296e+02  5.03142586e+02]]</t>
+          <t>[[5.59835602e+03 4.03820648e+03 1.62546085e+03 4.55098682e+02
+  1.06599271e+02 1.96651233e+01 3.96632007e+00]
+ [4.03820648e+03 5.59835509e+03 4.03820557e+03 1.62545995e+03
+  4.55097642e+02 1.06598512e+02 1.96645285e+01]
+ [1.62546085e+03 4.03820557e+03 5.59835452e+03 4.03820494e+03
+  1.62545882e+03 4.55097064e+02 1.06598321e+02]
+ [4.55098682e+02 1.62545995e+03 4.03820494e+03 5.59835383e+03
+  4.03820385e+03 1.62545821e+03 4.55096776e+02]
+ [1.06599271e+02 4.55097642e+02 1.62545882e+03 4.03820385e+03
+  5.59835272e+03 4.03820295e+03 1.62545740e+03]
+ [1.96651233e+01 1.06598512e+02 4.55097064e+02 1.62545821e+03
+  4.03820295e+03 5.59835219e+03 4.03820266e+03]
+ [3.96632007e+00 1.96645285e+01 1.06598321e+02 4.55096776e+02
+  1.62545740e+03 4.03820266e+03 5.59835228e+03]]</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>20.00055902852358</v>
+        <v>20.00055984497986</v>
       </c>
       <c r="E4" t="n">
-        <v>28.69137933855449</v>
+        <v>28.18275706525969</v>
       </c>
     </row>
     <row r="5">
@@ -568,32 +568,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[-0.15107749697392545, 0.14395420064686185, -1.0199135124499774, 2.19982973068618, -1.4696038891478476, 0.6956192782245417, -0.39880831098583314]</t>
+          <t>[-0.18276348567658302, 0.25604263882641604, -1.161775868493083, 2.3600693572697904, -1.685296905555232, 0.869155752201776, -0.4554314885730847]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[[ 7.07173395e+02  5.10835430e+02  2.03794986e+02  5.18478822e+01
-   7.51210301e+00 -4.07658239e-01 -3.65252170e-02]
- [ 5.10835430e+02  7.15773718e+02  5.09387044e+02  2.01515524e+02
-   5.34959771e+01  8.54883841e+00 -1.26233243e+00]
- [ 2.03794986e+02  5.09387044e+02  7.09226218e+02  5.08045445e+02
-   2.01809872e+02  5.24249870e+01  7.20557884e+00]
- [ 5.18478822e+01  2.01515524e+02  5.08045445e+02  7.13721849e+02
-   5.13529917e+02  2.02576542e+02  5.08464802e+01]
- [ 7.51210301e+00  5.34959771e+01  2.01809872e+02  5.13529917e+02
-   7.21784803e+02  5.11731551e+02  1.97562541e+02]
- [-4.07658239e-01  8.54883841e+00  5.24249870e+01  2.02576542e+02
-   5.11731551e+02  7.10106041e+02  5.03460624e+02]
- [-3.65252170e-02 -1.26233243e+00  7.20557884e+00  5.08464802e+01
-   1.97562541e+02  5.03460624e+02  7.07724279e+02]]</t>
+          <t>[[ 7.92776117e+03  5.71286771e+03  2.28823112e+03  6.28533915e+02
+   1.32709092e+02  1.08934192e+01 -3.30821265e+00]
+ [ 5.71286771e+03  7.92775895e+03  5.71286560e+03  2.28822867e+03
+   6.28531243e+02  1.32706720e+02  1.08917366e+01]
+ [ 2.28823112e+03  5.71286560e+03  7.92775730e+03  5.71286269e+03
+   2.28822412e+03  6.28528128e+02  1.32705513e+02]
+ [ 6.28533915e+02  2.28822867e+03  5.71286269e+03  7.92775551e+03
+   5.71286295e+03  2.28822288e+03  6.28525641e+02]
+ [ 1.32709092e+02  6.28531243e+02  2.28822412e+03  5.71286295e+03
+   7.92776347e+03  5.71286488e+03  2.28821866e+03]
+ [ 1.08934192e+01  1.32706720e+02  6.28528128e+02  2.28822288e+03
+   5.71286488e+03  7.92776299e+03  5.71286215e+03]
+ [-3.30821265e+00  1.08917366e+01  1.32705513e+02  6.28525641e+02
+   2.28821866e+03  5.71286215e+03  7.92776214e+03]]</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>30.03758037555496</v>
+        <v>30.03758116519379</v>
       </c>
       <c r="E5" t="n">
-        <v>34.04036099469235</v>
+        <v>33.61435739698369</v>
       </c>
     </row>
     <row r="6">
@@ -602,32 +602,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[-0.14952753315459036, 0.14524883604941738, -1.0289050057324118, 2.2105101993677145, -1.4833859808145358, 0.7025099711730591, -0.3964504868886532]</t>
+          <t>[-0.18192125478375493, 0.2523048657972979, -1.1567808388968905, 2.35439629041872, -1.6775691708081966, 0.8626153743069531, -0.45304526603412903]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[[ 8.93082432e+02  6.36494911e+02  2.52252449e+02  6.63873200e+01
-   1.04063409e+01 -2.12476845e+00 -8.25011634e-01]
- [ 6.36494911e+02  8.80648023e+02  6.34088262e+02  2.53267862e+02
-   6.60193857e+01  8.25506187e+00 -2.69434481e+00]
- [ 2.52252449e+02  6.34088262e+02  8.96678486e+02  6.41100195e+02
-   2.52652118e+02  6.37363901e+01  9.45689599e+00]
- [ 6.63873200e+01  2.53267862e+02  6.41100195e+02  8.92618237e+02
-   6.38987648e+02  2.50655347e+02  6.44440354e+01]
- [ 1.04063409e+01  6.60193857e+01  2.52652118e+02  6.38987648e+02
-   8.92646024e+02  6.33435711e+02  2.50491950e+02]
- [-2.12476845e+00  8.25506187e+00  6.37363901e+01  2.50655347e+02
-   6.33435711e+02  8.83313374e+02  6.33541253e+02]
- [-8.25011634e-01 -2.69434481e+00  9.45689599e+00  6.44440354e+01
-   2.50491950e+02  6.33541253e+02  8.86006026e+02]]</t>
+          <t>[[ 9.96858601e+03  7.18903851e+03  2.89247868e+03  8.04844412e+02
+   1.72576899e+02  1.40129085e+01 -7.11914974e+00]
+ [ 7.18903851e+03  9.96858252e+03  7.18903558e+03  2.89247556e+03
+   8.04840864e+02  1.72573658e+02  1.40155439e+01]
+ [ 2.89247868e+03  7.18903558e+03  9.96858106e+03  7.18903433e+03
+   2.89247272e+03  8.04836423e+02  1.72576006e+02]
+ [ 8.04844412e+02  2.89247556e+03  7.18903433e+03  9.96858013e+03
+   7.18903134e+03  2.89246748e+03  8.04838963e+02]
+ [ 1.72576899e+02  8.04840864e+02  2.89247272e+03  7.18903134e+03
+   9.96857654e+03  7.18902781e+03  2.89247018e+03]
+ [ 1.40129085e+01  1.72573658e+02  8.04836423e+02  2.89246748e+03
+   7.18902781e+03  9.96857647e+03  7.18903003e+03]
+ [-7.11914974e+00  1.40155439e+01  1.72576006e+02  8.04838963e+02
+   2.89247018e+03  7.18903003e+03  9.96857449e+03]]</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>40.03604706152543</v>
+        <v>40.03604063705254</v>
       </c>
       <c r="E6" t="n">
-        <v>38.27546277079185</v>
+        <v>37.86708063944564</v>
       </c>
     </row>
     <row r="7">
@@ -636,32 +636,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[-0.1562909108046308, 0.15428518860541718, -1.0358630872615902, 2.217763291130791, -1.4908608555757894, 0.7001014115545262, -0.3891350376487244]</t>
+          <t>[-0.1828681809914243, 0.2542734350391428, -1.158327630239351, 2.356087062113949, -1.6800084877969743, 0.8653758991619164, -0.45453209728725874]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[[1048.196394    749.88831109  300.79722095   84.86655354   18.9606472
-     1.95072729    3.64117086]
- [ 749.88831109 1051.9624322   754.25831681  305.17716399   84.43076986
-    14.58634162    4.21691832]
- [ 300.79722095  754.25831681 1051.08305699  754.41871051  300.90570937
-    77.056274     12.05011216]
- [  84.86655354  305.17716399  754.41871051 1051.50174454  754.92539775
-   298.62574415   73.57008669]
- [  18.9606472    84.43076986  300.90570937  754.92539775 1053.237859
-   751.5202203   293.40866212]
- [   1.95072729   14.58634162   77.056274    298.62574415  751.5202203
-  1047.88283628  749.04017586]
- [   3.64117086    4.21691832   12.05011216   73.57008669  293.40866212
-   749.04017586 1048.45628792]]</t>
+          <t>[[11676.67477403  8407.46567598  3358.23135467   917.07530494
+    193.68138815    26.0402384     15.77905971]
+ [ 8407.46567598 11676.66967216  8407.4612414   3358.22526237
+    917.06732334   193.6739336     26.0408018 ]
+ [ 3358.23135467  8407.4612414  11676.66594091  8407.45531368
+   3358.21683302   917.05918267   193.67362244]
+ [  917.07530494  3358.22526237  8407.45531368 11676.66190731
+   8407.45343014  3358.21644752   917.06396141]
+ [  193.68138815   917.06732334  3358.21683302  8407.45343014
+  11676.6674636   8407.46186045  3358.22701626]
+ [   26.0402384    193.6739336    917.05918267  3358.21644752
+   8407.46186045 11676.67894626  8407.47347134]
+ [   15.77905971    26.0408018    193.67362244   917.06396141
+   3358.22701626  8407.47347134 11676.68408516]]</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>50.0257592924174</v>
+        <v>50.02575699870505</v>
       </c>
       <c r="E7" t="n">
-        <v>41.73221539559243</v>
+        <v>41.33406067433952</v>
       </c>
     </row>
     <row r="8">
@@ -670,32 +670,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[-0.15618573599266114, 0.1492985315254396, -1.0201245743586893, 2.199506662660773, -1.4687800088778589, 0.6945423285209582, -0.3982572034779615]</t>
+          <t>[-0.18308082403075995, 0.2505735875242717, -1.1511835167552298, 2.347851649566885, -1.6691723465727377, 0.8579893003733295, -0.45297785010575936]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[[1184.26267829  843.506856    333.93307671   89.45748569   16.89030475
-     4.11783885    2.87786948]
- [ 843.506856   1167.30116479  832.45075328  329.12229908   87.49374241
-    17.45230647    2.33505595]
- [ 333.93307671  832.45075328 1162.37166973  828.89594486  328.40671558
-    89.884902     16.85568672]
- [  89.45748569  329.12229908  828.89594486 1159.25472713  832.3229607
-   335.41697212   91.70685641]
- [  16.89030475   87.49374241  328.40671558  832.3229607  1170.97597617
-   842.12899164  336.09170102]
- [   4.11783885   17.45230647   89.884902    335.41697212  842.12899164
-  1174.32340923  839.30652075]
- [   2.87786948    2.33505595   16.85568672   91.70685641  336.09170102
-   839.30652075 1171.77523899]]</t>
+          <t>[[ 1.30767820e+04  9.41373564e+03  3.76490225e+03  1.03458575e+03
+   2.11683334e+02  1.11563415e+01 -2.33903678e+00]
+ [ 9.41373564e+03  1.30767742e+04  9.41372787e+03  3.76489344e+03
+   1.03457822e+03  2.11676868e+02  1.11564950e+01]
+ [ 3.76490225e+03  9.41372787e+03  1.30767670e+04  9.41372020e+03
+   3.76488563e+03  1.03457148e+03  2.11677782e+02]
+ [ 1.03458575e+03  3.76489344e+03  9.41372020e+03  1.30767594e+04
+   9.41371100e+03  3.76487765e+03  1.03457332e+03]
+ [ 2.11683334e+02  1.03457822e+03  3.76488563e+03  9.41371100e+03
+   1.30767524e+04  9.41370500e+03  3.76487730e+03]
+ [ 1.11563415e+01  2.11676868e+02  1.03457148e+03  3.76487765e+03
+   9.41370500e+03  1.30767473e+04  9.41370464e+03]
+ [-2.33903678e+00  1.11564950e+01  2.11677782e+02  1.03457332e+03
+   3.76487730e+03  9.41370464e+03  1.30767484e+04]]</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>60.03490151692988</v>
+        <v>60.03489893313372</v>
       </c>
       <c r="E8" t="n">
-        <v>44.56947361368592</v>
+        <v>44.0959034346501</v>
       </c>
     </row>
     <row r="9">
@@ -704,32 +704,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[-0.15809240543350678, 0.14567815525649064, -1.0190222941569569, 2.1986350921874913, -1.4682045719693286, 0.6937116248406134, -0.392705600724803]</t>
+          <t>[-0.1839726850727479, 0.2498368586898096, -1.1481797628613974, 2.3443328488293007, -1.6647612399934575, 0.8559675364228486, -0.45322355601435593]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[[1285.03303403  923.9361939   375.38241416  109.25758422   24.57777442
-     6.63020292    6.33275142]
- [ 923.9361939  1285.27249011  922.04091769  374.5160219   105.3683808
-    22.28476987    6.39215277]
- [ 375.38241416  922.04091769 1279.47654473  919.45162891  370.64351862
-   102.98139894   21.23839477]
- [ 109.25758422  374.5160219   919.45162891 1282.18178535  914.73592833
-   362.20265153   96.64457905]
- [  24.57777442  105.3683808   370.64351862  914.73592833 1268.61411627
-   905.09126204  360.83405998]
- [   6.63020292   22.28476987  102.98139894  362.20265153  905.09126204
-  1265.00025492  905.48469548]
- [   6.33275142    6.39215277   21.23839477   96.64457905  360.83405998
-   905.48469548 1266.22455008]]</t>
+          <t>[[1.41741922e+04 1.01999188e+04 4.07901741e+03 1.13084379e+03
+  2.47564069e+02 2.82141715e+01 1.86582650e+00]
+ [1.01999188e+04 1.41741815e+04 1.01999080e+04 4.07900561e+03
+  1.13083346e+03 2.47556096e+02 2.82146178e+01]
+ [4.07901741e+03 1.01999080e+04 1.41741718e+04 1.01998979e+04
+  4.07899373e+03 1.13082212e+03 2.47555294e+02]
+ [1.13084379e+03 4.07900561e+03 1.01998979e+04 1.41741616e+04
+  1.01998844e+04 4.07898011e+03 1.13082076e+03]
+ [2.47564069e+02 1.13083346e+03 4.07899373e+03 1.01998844e+04
+  1.41741530e+04 1.01998802e+04 4.07898190e+03]
+ [2.82141715e+01 2.47556096e+02 1.13082212e+03 4.07898011e+03
+  1.01998802e+04 1.41741553e+04 1.01998837e+04]
+ [1.86582650e+00 2.82146178e+01 2.47555294e+02 1.13082076e+03
+  4.07898190e+03 1.01998837e+04 1.41741565e+04]]</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>70.00550113122169</v>
+        <v>70.0054989833304</v>
       </c>
       <c r="E9" t="n">
-        <v>46.85559589062421</v>
+        <v>46.37619586234757</v>
       </c>
     </row>
     <row r="10">
@@ -738,32 +738,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[-0.16021354550189745, 0.15079333435534142, -1.0188586502141912, 2.197802232069211, -1.4661630663559964, 0.6909606637071483, -0.39432096805961586]</t>
+          <t>[-0.18532961528993877, 0.24931478829528445, -1.144487808391345, 2.3399756580396316, -1.6593548982593382, 0.8538326224463995, -0.4539507468406927]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[[ 1.35152797e+03  9.68158579e+02  3.87131135e+02  1.10357698e+02
-   2.53635434e+01 -1.95853398e+00 -6.29538202e+00]
- [ 9.68158579e+02  1.35329129e+03  9.66948179e+02  3.90075523e+02
-   1.12040996e+02  2.25674829e+01  1.31919831e+00]
- [ 3.87131135e+02  9.66948179e+02  1.35293569e+03  9.74084590e+02
-   3.91914745e+02  1.11094266e+02  2.58041287e+01]
- [ 1.10357698e+02  3.90075523e+02  9.74084590e+02  1.36300450e+03
-   9.72767958e+02  3.87471643e+02  1.06484250e+02]
- [ 2.53635434e+01  1.12040996e+02  3.91914745e+02  9.72767958e+02
-   1.34933411e+03  9.60508188e+02  3.83540750e+02]
- [-1.95853398e+00  2.25674829e+01  1.11094266e+02  3.87471643e+02
-   9.60508188e+02  1.34374085e+03  9.67795582e+02]
- [-6.29538202e+00  1.31919831e+00  2.58041287e+01  1.06484250e+02
-   3.83540750e+02  9.67795582e+02  1.35671661e+03]]</t>
+          <t>[[1.49553721e+04 1.07480515e+04 4.28125487e+03 1.18406291e+03
+  2.64632550e+02 3.66482702e+01 1.00470091e+01]
+ [1.07480515e+04 1.49553573e+04 1.07480389e+04 4.28125358e+03
+  1.18407256e+03 2.64629170e+02 3.66353134e+01]
+ [4.28125487e+03 1.07480389e+04 1.49553466e+04 1.07480379e+04
+  4.28126174e+03 1.18406967e+03 2.64618175e+02]
+ [1.18406291e+03 4.28125358e+03 1.07480379e+04 1.49553470e+04
+  1.07480395e+04 4.28125936e+03 1.18406528e+03]
+ [2.64632550e+02 1.18407256e+03 4.28126174e+03 1.07480395e+04
+  1.49553422e+04 1.07480382e+04 4.28126220e+03]
+ [3.66482702e+01 2.64629170e+02 1.18406967e+03 4.28125936e+03
+  1.07480382e+04 1.49553502e+04 1.07480491e+04]
+ [1.00470091e+01 3.66353134e+01 2.64618175e+02 1.18406528e+03
+  4.28126220e+03 1.07480491e+04 1.49553607e+04]]</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>80.00328769999282</v>
+        <v>80.00328588728216</v>
       </c>
       <c r="E10" t="n">
-        <v>48.66085315520022</v>
+        <v>48.20270486128138</v>
       </c>
     </row>
     <row r="11">
@@ -772,32 +772,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[-0.16426076541053306, 0.1498625228543782, -1.0126931093502356, 2.1905707007253246, -1.4574340812328686, 0.6877330658125881, -0.3937783333986534]</t>
+          <t>[-0.1845783017392161, 0.24630276136623444, -1.1405681530694103, 2.3355301791739147, -1.6532857932168252, 0.8486370169125382, -0.4520377094272355]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[[1388.87972822  993.15858709  391.35253583  106.62740336   21.46542105
-     8.19264178   10.43283213]
- [ 993.15858709 1398.4908516   994.51743554  394.54579604  109.90962712
-    28.8681358    10.42915243]
- [ 391.35253583  994.51743554 1383.70076086  988.27430828  394.49851005
-   109.35345994   22.14073784]
- [ 106.62740336  394.54579604  988.27430828 1384.33844294  985.48080484
-   387.60759409  101.49363777]
- [  21.46542105  109.90962712  394.49851005  985.48080484 1374.81480376
-   981.57373165  387.813493  ]
- [   8.19264178   28.8681358   109.35345994  387.60759409  981.57373165
-  1376.26526497  977.5417714 ]
- [  10.43283213   10.42915243   22.14073784  101.49363777  387.813493
-   977.5417714  1367.2961736 ]]</t>
+          <t>[[15455.49666257 11103.3582555   4417.34475876  1214.55200594
+    264.89457627    37.51061259    16.9382566 ]
+ [11103.3582555  15455.48534289 11103.35608072  4417.34907071
+   1214.54635485   264.88042106    37.49684571]
+ [ 4417.34475876 11103.35608072 15455.48499571 11103.35665099
+   4417.34749358  1214.54294687   264.87675004]
+ [ 1214.55200594  4417.34907071 11103.35665099 15455.48429649
+  11103.36059927  4417.35540117  1214.55194032]
+ [  264.89457627  1214.54635485  4417.34749358 11103.36059927
+  15455.48489343 11103.35832108  4417.35566544]
+ [   37.51061259   264.88042106  1214.54294687  4417.35540117
+  11103.35832108 15455.47390064 11103.35110404]
+ [   16.9382566     37.49684571   264.87675004  1214.55194032
+   4417.35566544 11103.35110404 15455.47205976]]</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>89.97546387337403</v>
+        <v>89.97546200833011</v>
       </c>
       <c r="E11" t="n">
-        <v>50.11089492235458</v>
+        <v>49.64993635226323</v>
       </c>
     </row>
     <row r="12">
@@ -806,32 +806,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[-0.1546366364243046, 0.1368208435863422, -1.0048635288335752, 2.1826657148992132, -1.4490644720845063, 0.6884704831006482, -0.3993924042438173]</t>
+          <t>[-0.184837425491477, 0.24078242060484187, -1.1301364837833565, 2.323512101190851, -1.6374286424214453, 0.8376126647110799, -0.44950463481049363]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[[1.42356732e+03 1.01476552e+03 4.00153937e+02 1.08005506e+02
-  1.92800593e+01 1.30707030e-01 4.45408280e+00]
- [1.01476552e+03 1.41115758e+03 1.00029932e+03 3.93188952e+02
-  9.98419684e+01 1.51027773e+01 1.39367078e+00]
- [4.00153937e+02 1.00029932e+03 1.40216904e+03 9.97914229e+02
-  3.87136156e+02 9.84108988e+01 1.70033225e+01]
- [1.08005506e+02 3.93188952e+02 9.97914229e+02 1.39690209e+03
-  9.93545651e+02 3.91116632e+02 1.06214275e+02]
- [1.92800593e+01 9.98419684e+01 3.87136156e+02 9.93545651e+02
-  1.40458818e+03 1.00813233e+03 4.00299782e+02]
- [1.30707030e-01 1.51027773e+01 9.84108988e+01 3.91116632e+02
-  1.00813233e+03 1.41420244e+03 1.00656048e+03]
- [4.45408280e+00 1.39367078e+00 1.70033225e+01 1.06214275e+02
-  4.00299782e+02 1.00656048e+03 1.41223743e+03]]</t>
+          <t>[[15600.26605801 11189.66364836  4432.15999305  1207.89595176
+    253.99792299    32.76878168    17.19411474]
+ [11189.66364836 15600.24842915 11189.66241284  4432.17053028
+   1207.89186249   253.98926769    32.76406083]
+ [ 4432.15999305 11189.66241284 15600.30139449 11189.71531053
+   4432.19121682  1207.90879195   253.99485369]
+ [ 1207.89595176  4432.17053028 11189.71531053 15600.34637759
+  11189.738375    4432.21363129  1207.91743102]
+ [  253.99792299  1207.89186249  4432.19121682 11189.738375
+  15600.35372038 11189.74329985  4432.21487535]
+ [   32.76878168   253.98926769  1207.90879195  4432.21363129
+  11189.74329985 15600.35526732 11189.74293783]
+ [   17.19411474    32.76406083   253.99485369  1207.91743102
+   4432.21487535 11189.74293783 15600.35466302]]</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>99.9237204068171</v>
+        <v>99.92372534861725</v>
       </c>
       <c r="E12" t="n">
-        <v>51.13829918391575</v>
+        <v>50.69647530797238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>